<commit_message>
Update mau_kegio.xlsx to reflect recent data changes
</commit_message>
<xml_diff>
--- a/data_base/mau_kegio.xlsx
+++ b/data_base/mau_kegio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E77506-1821-481D-B7B9-3541F861FE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0420F39C-82E5-453B-9F2C-514AE20042D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hướng dẫn" sheetId="1" r:id="rId1"/>
@@ -2645,7 +2645,7 @@
     <xf numFmtId="172" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="319">
+  <cellXfs count="318">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3627,9 +3627,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="76" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -3641,6 +3638,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -3678,10 +3678,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="79" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -15181,7 +15177,7 @@
       <c r="J63" s="131"/>
       <c r="K63" s="131"/>
       <c r="L63" s="153">
-        <f t="shared" ref="L44:L71" si="2">(G63*I63+H63*J63)*E63</f>
+        <f t="shared" ref="L63:L71" si="2">(G63*I63+H63*J63)*E63</f>
         <v>0</v>
       </c>
     </row>
@@ -15472,7 +15468,7 @@
       <c r="D78" s="222"/>
       <c r="E78" s="130"/>
       <c r="F78" s="151">
-        <f t="shared" ref="F76:F107" si="5">SUM(G78,H78)</f>
+        <f t="shared" ref="F78:F107" si="5">SUM(G78,H78)</f>
         <v>0</v>
       </c>
       <c r="G78" s="128"/>
@@ -18327,7 +18323,7 @@
   <dimension ref="A1:M244"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -18478,7 +18474,7 @@
       <c r="C8" s="21"/>
       <c r="D8" s="220"/>
       <c r="E8" s="130"/>
-      <c r="F8" s="318">
+      <c r="F8" s="151">
         <f>SUM(G8,H8)</f>
         <v>0</v>
       </c>
@@ -18498,7 +18494,7 @@
       <c r="C9" s="21"/>
       <c r="D9" s="220"/>
       <c r="E9" s="130"/>
-      <c r="F9" s="318">
+      <c r="F9" s="151">
         <f t="shared" ref="F9:F72" si="0">SUM(G9,H9)</f>
         <v>0</v>
       </c>
@@ -18518,7 +18514,7 @@
       <c r="C10" s="21"/>
       <c r="D10" s="220"/>
       <c r="E10" s="130"/>
-      <c r="F10" s="318">
+      <c r="F10" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18538,7 +18534,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="220"/>
       <c r="E11" s="130"/>
-      <c r="F11" s="318">
+      <c r="F11" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18558,7 +18554,7 @@
       <c r="C12" s="21"/>
       <c r="D12" s="220"/>
       <c r="E12" s="130"/>
-      <c r="F12" s="318">
+      <c r="F12" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18578,7 +18574,7 @@
       <c r="C13" s="21"/>
       <c r="D13" s="220"/>
       <c r="E13" s="130"/>
-      <c r="F13" s="318">
+      <c r="F13" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18598,7 +18594,7 @@
       <c r="C14" s="21"/>
       <c r="D14" s="220"/>
       <c r="E14" s="130"/>
-      <c r="F14" s="318">
+      <c r="F14" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18618,7 +18614,7 @@
       <c r="C15" s="21"/>
       <c r="D15" s="220"/>
       <c r="E15" s="130"/>
-      <c r="F15" s="318">
+      <c r="F15" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18638,7 +18634,7 @@
       <c r="C16" s="21"/>
       <c r="D16" s="220"/>
       <c r="E16" s="130"/>
-      <c r="F16" s="318">
+      <c r="F16" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18658,7 +18654,7 @@
       <c r="C17" s="21"/>
       <c r="D17" s="220"/>
       <c r="E17" s="130"/>
-      <c r="F17" s="318">
+      <c r="F17" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18678,7 +18674,7 @@
       <c r="C18" s="21"/>
       <c r="D18" s="220"/>
       <c r="E18" s="130"/>
-      <c r="F18" s="318">
+      <c r="F18" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18698,7 +18694,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="220"/>
       <c r="E19" s="130"/>
-      <c r="F19" s="318">
+      <c r="F19" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18718,7 +18714,7 @@
       <c r="C20" s="21"/>
       <c r="D20" s="220"/>
       <c r="E20" s="130"/>
-      <c r="F20" s="318">
+      <c r="F20" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18738,7 +18734,7 @@
       <c r="C21" s="21"/>
       <c r="D21" s="220"/>
       <c r="E21" s="130"/>
-      <c r="F21" s="318">
+      <c r="F21" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18758,7 +18754,7 @@
       <c r="C22" s="21"/>
       <c r="D22" s="220"/>
       <c r="E22" s="130"/>
-      <c r="F22" s="318">
+      <c r="F22" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18778,7 +18774,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="220"/>
       <c r="E23" s="130"/>
-      <c r="F23" s="318">
+      <c r="F23" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18798,7 +18794,7 @@
       <c r="C24" s="21"/>
       <c r="D24" s="220"/>
       <c r="E24" s="130"/>
-      <c r="F24" s="318">
+      <c r="F24" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18818,7 +18814,7 @@
       <c r="C25" s="21"/>
       <c r="D25" s="220"/>
       <c r="E25" s="130"/>
-      <c r="F25" s="318">
+      <c r="F25" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18838,7 +18834,7 @@
       <c r="C26" s="21"/>
       <c r="D26" s="220"/>
       <c r="E26" s="130"/>
-      <c r="F26" s="318">
+      <c r="F26" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18858,7 +18854,7 @@
       <c r="C27" s="21"/>
       <c r="D27" s="220"/>
       <c r="E27" s="130"/>
-      <c r="F27" s="318">
+      <c r="F27" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18878,7 +18874,7 @@
       <c r="C28" s="21"/>
       <c r="D28" s="220"/>
       <c r="E28" s="130"/>
-      <c r="F28" s="318">
+      <c r="F28" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18898,7 +18894,7 @@
       <c r="C29" s="21"/>
       <c r="D29" s="220"/>
       <c r="E29" s="130"/>
-      <c r="F29" s="318">
+      <c r="F29" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18918,7 +18914,7 @@
       <c r="C30" s="21"/>
       <c r="D30" s="220"/>
       <c r="E30" s="130"/>
-      <c r="F30" s="318">
+      <c r="F30" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18938,7 +18934,7 @@
       <c r="C31" s="21"/>
       <c r="D31" s="220"/>
       <c r="E31" s="130"/>
-      <c r="F31" s="318">
+      <c r="F31" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18958,7 +18954,7 @@
       <c r="C32" s="21"/>
       <c r="D32" s="220"/>
       <c r="E32" s="130"/>
-      <c r="F32" s="318">
+      <c r="F32" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18978,7 +18974,7 @@
       <c r="C33" s="21"/>
       <c r="D33" s="220"/>
       <c r="E33" s="130"/>
-      <c r="F33" s="318">
+      <c r="F33" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -18998,7 +18994,7 @@
       <c r="C34" s="21"/>
       <c r="D34" s="220"/>
       <c r="E34" s="130"/>
-      <c r="F34" s="318">
+      <c r="F34" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19018,7 +19014,7 @@
       <c r="C35" s="21"/>
       <c r="D35" s="220"/>
       <c r="E35" s="130"/>
-      <c r="F35" s="318">
+      <c r="F35" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19038,7 +19034,7 @@
       <c r="C36" s="21"/>
       <c r="D36" s="220"/>
       <c r="E36" s="130"/>
-      <c r="F36" s="318">
+      <c r="F36" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19058,7 +19054,7 @@
       <c r="C37" s="21"/>
       <c r="D37" s="220"/>
       <c r="E37" s="130"/>
-      <c r="F37" s="318">
+      <c r="F37" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19078,7 +19074,7 @@
       <c r="C38" s="21"/>
       <c r="D38" s="220"/>
       <c r="E38" s="130"/>
-      <c r="F38" s="318">
+      <c r="F38" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19098,7 +19094,7 @@
       <c r="C39" s="21"/>
       <c r="D39" s="220"/>
       <c r="E39" s="130"/>
-      <c r="F39" s="318">
+      <c r="F39" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19118,7 +19114,7 @@
       <c r="C40" s="21"/>
       <c r="D40" s="220"/>
       <c r="E40" s="130"/>
-      <c r="F40" s="318">
+      <c r="F40" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19138,7 +19134,7 @@
       <c r="C41" s="21"/>
       <c r="D41" s="220"/>
       <c r="E41" s="130"/>
-      <c r="F41" s="318">
+      <c r="F41" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19158,7 +19154,7 @@
       <c r="C42" s="21"/>
       <c r="D42" s="220"/>
       <c r="E42" s="130"/>
-      <c r="F42" s="318">
+      <c r="F42" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19178,7 +19174,7 @@
       <c r="C43" s="21"/>
       <c r="D43" s="220"/>
       <c r="E43" s="130"/>
-      <c r="F43" s="318">
+      <c r="F43" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19198,7 +19194,7 @@
       <c r="C44" s="21"/>
       <c r="D44" s="220"/>
       <c r="E44" s="130"/>
-      <c r="F44" s="318">
+      <c r="F44" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19218,7 +19214,7 @@
       <c r="C45" s="21"/>
       <c r="D45" s="220"/>
       <c r="E45" s="130"/>
-      <c r="F45" s="318">
+      <c r="F45" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19238,7 +19234,7 @@
       <c r="C46" s="21"/>
       <c r="D46" s="220"/>
       <c r="E46" s="130"/>
-      <c r="F46" s="318">
+      <c r="F46" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19258,7 +19254,7 @@
       <c r="C47" s="21"/>
       <c r="D47" s="220"/>
       <c r="E47" s="130"/>
-      <c r="F47" s="318">
+      <c r="F47" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19278,7 +19274,7 @@
       <c r="C48" s="21"/>
       <c r="D48" s="220"/>
       <c r="E48" s="130"/>
-      <c r="F48" s="318">
+      <c r="F48" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19298,7 +19294,7 @@
       <c r="C49" s="21"/>
       <c r="D49" s="220"/>
       <c r="E49" s="130"/>
-      <c r="F49" s="318">
+      <c r="F49" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19318,7 +19314,7 @@
       <c r="C50" s="21"/>
       <c r="D50" s="220"/>
       <c r="E50" s="130"/>
-      <c r="F50" s="318">
+      <c r="F50" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19338,7 +19334,7 @@
       <c r="C51" s="21"/>
       <c r="D51" s="220"/>
       <c r="E51" s="130"/>
-      <c r="F51" s="318">
+      <c r="F51" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19358,7 +19354,7 @@
       <c r="C52" s="21"/>
       <c r="D52" s="220"/>
       <c r="E52" s="130"/>
-      <c r="F52" s="318">
+      <c r="F52" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19378,7 +19374,7 @@
       <c r="C53" s="21"/>
       <c r="D53" s="220"/>
       <c r="E53" s="130"/>
-      <c r="F53" s="318">
+      <c r="F53" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19398,7 +19394,7 @@
       <c r="C54" s="21"/>
       <c r="D54" s="220"/>
       <c r="E54" s="130"/>
-      <c r="F54" s="318">
+      <c r="F54" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19418,7 +19414,7 @@
       <c r="C55" s="21"/>
       <c r="D55" s="220"/>
       <c r="E55" s="130"/>
-      <c r="F55" s="318">
+      <c r="F55" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19438,7 +19434,7 @@
       <c r="C56" s="21"/>
       <c r="D56" s="220"/>
       <c r="E56" s="130"/>
-      <c r="F56" s="318">
+      <c r="F56" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19458,7 +19454,7 @@
       <c r="C57" s="21"/>
       <c r="D57" s="220"/>
       <c r="E57" s="130"/>
-      <c r="F57" s="318">
+      <c r="F57" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19478,7 +19474,7 @@
       <c r="C58" s="21"/>
       <c r="D58" s="220"/>
       <c r="E58" s="130"/>
-      <c r="F58" s="318">
+      <c r="F58" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19498,7 +19494,7 @@
       <c r="C59" s="21"/>
       <c r="D59" s="220"/>
       <c r="E59" s="130"/>
-      <c r="F59" s="318">
+      <c r="F59" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19518,7 +19514,7 @@
       <c r="C60" s="21"/>
       <c r="D60" s="220"/>
       <c r="E60" s="130"/>
-      <c r="F60" s="318">
+      <c r="F60" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19538,7 +19534,7 @@
       <c r="C61" s="21"/>
       <c r="D61" s="220"/>
       <c r="E61" s="130"/>
-      <c r="F61" s="318">
+      <c r="F61" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19558,7 +19554,7 @@
       <c r="C62" s="21"/>
       <c r="D62" s="220"/>
       <c r="E62" s="130"/>
-      <c r="F62" s="318">
+      <c r="F62" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19578,7 +19574,7 @@
       <c r="C63" s="21"/>
       <c r="D63" s="220"/>
       <c r="E63" s="130"/>
-      <c r="F63" s="318">
+      <c r="F63" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19598,7 +19594,7 @@
       <c r="C64" s="21"/>
       <c r="D64" s="220"/>
       <c r="E64" s="130"/>
-      <c r="F64" s="318">
+      <c r="F64" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19618,7 +19614,7 @@
       <c r="C65" s="21"/>
       <c r="D65" s="220"/>
       <c r="E65" s="130"/>
-      <c r="F65" s="318">
+      <c r="F65" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19638,7 +19634,7 @@
       <c r="C66" s="21"/>
       <c r="D66" s="220"/>
       <c r="E66" s="130"/>
-      <c r="F66" s="318">
+      <c r="F66" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19658,7 +19654,7 @@
       <c r="C67" s="21"/>
       <c r="D67" s="220"/>
       <c r="E67" s="130"/>
-      <c r="F67" s="318">
+      <c r="F67" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19678,7 +19674,7 @@
       <c r="C68" s="21"/>
       <c r="D68" s="220"/>
       <c r="E68" s="130"/>
-      <c r="F68" s="318">
+      <c r="F68" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19698,7 +19694,7 @@
       <c r="C69" s="21"/>
       <c r="D69" s="220"/>
       <c r="E69" s="130"/>
-      <c r="F69" s="318">
+      <c r="F69" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19718,7 +19714,7 @@
       <c r="C70" s="21"/>
       <c r="D70" s="220"/>
       <c r="E70" s="130"/>
-      <c r="F70" s="318">
+      <c r="F70" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19738,7 +19734,7 @@
       <c r="C71" s="21"/>
       <c r="D71" s="220"/>
       <c r="E71" s="130"/>
-      <c r="F71" s="318">
+      <c r="F71" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19758,7 +19754,7 @@
       <c r="C72" s="21"/>
       <c r="D72" s="220"/>
       <c r="E72" s="130"/>
-      <c r="F72" s="318">
+      <c r="F72" s="151">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -19778,7 +19774,7 @@
       <c r="C73" s="21"/>
       <c r="D73" s="220"/>
       <c r="E73" s="130"/>
-      <c r="F73" s="318">
+      <c r="F73" s="151">
         <f t="shared" ref="F73:F136" si="2">SUM(G73,H73)</f>
         <v>0</v>
       </c>
@@ -19798,7 +19794,7 @@
       <c r="C74" s="21"/>
       <c r="D74" s="220"/>
       <c r="E74" s="130"/>
-      <c r="F74" s="318">
+      <c r="F74" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19818,7 +19814,7 @@
       <c r="C75" s="21"/>
       <c r="D75" s="220"/>
       <c r="E75" s="130"/>
-      <c r="F75" s="318">
+      <c r="F75" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19838,7 +19834,7 @@
       <c r="C76" s="21"/>
       <c r="D76" s="220"/>
       <c r="E76" s="130"/>
-      <c r="F76" s="318">
+      <c r="F76" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19858,7 +19854,7 @@
       <c r="C77" s="21"/>
       <c r="D77" s="220"/>
       <c r="E77" s="130"/>
-      <c r="F77" s="318">
+      <c r="F77" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19878,7 +19874,7 @@
       <c r="C78" s="21"/>
       <c r="D78" s="220"/>
       <c r="E78" s="130"/>
-      <c r="F78" s="318">
+      <c r="F78" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19898,7 +19894,7 @@
       <c r="C79" s="21"/>
       <c r="D79" s="220"/>
       <c r="E79" s="130"/>
-      <c r="F79" s="318">
+      <c r="F79" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19918,7 +19914,7 @@
       <c r="C80" s="21"/>
       <c r="D80" s="220"/>
       <c r="E80" s="130"/>
-      <c r="F80" s="318">
+      <c r="F80" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19938,7 +19934,7 @@
       <c r="C81" s="21"/>
       <c r="D81" s="220"/>
       <c r="E81" s="130"/>
-      <c r="F81" s="318">
+      <c r="F81" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19958,7 +19954,7 @@
       <c r="C82" s="21"/>
       <c r="D82" s="220"/>
       <c r="E82" s="130"/>
-      <c r="F82" s="318">
+      <c r="F82" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19978,7 +19974,7 @@
       <c r="C83" s="21"/>
       <c r="D83" s="220"/>
       <c r="E83" s="130"/>
-      <c r="F83" s="318">
+      <c r="F83" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -19998,7 +19994,7 @@
       <c r="C84" s="21"/>
       <c r="D84" s="220"/>
       <c r="E84" s="130"/>
-      <c r="F84" s="318">
+      <c r="F84" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20018,7 +20014,7 @@
       <c r="C85" s="21"/>
       <c r="D85" s="220"/>
       <c r="E85" s="130"/>
-      <c r="F85" s="318">
+      <c r="F85" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20038,7 +20034,7 @@
       <c r="C86" s="21"/>
       <c r="D86" s="220"/>
       <c r="E86" s="130"/>
-      <c r="F86" s="318">
+      <c r="F86" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20058,7 +20054,7 @@
       <c r="C87" s="21"/>
       <c r="D87" s="220"/>
       <c r="E87" s="130"/>
-      <c r="F87" s="318">
+      <c r="F87" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20078,7 +20074,7 @@
       <c r="C88" s="21"/>
       <c r="D88" s="220"/>
       <c r="E88" s="130"/>
-      <c r="F88" s="318">
+      <c r="F88" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20098,7 +20094,7 @@
       <c r="C89" s="21"/>
       <c r="D89" s="220"/>
       <c r="E89" s="130"/>
-      <c r="F89" s="318">
+      <c r="F89" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20118,7 +20114,7 @@
       <c r="C90" s="21"/>
       <c r="D90" s="220"/>
       <c r="E90" s="130"/>
-      <c r="F90" s="318">
+      <c r="F90" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20138,7 +20134,7 @@
       <c r="C91" s="21"/>
       <c r="D91" s="220"/>
       <c r="E91" s="130"/>
-      <c r="F91" s="318">
+      <c r="F91" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20158,7 +20154,7 @@
       <c r="C92" s="21"/>
       <c r="D92" s="220"/>
       <c r="E92" s="130"/>
-      <c r="F92" s="318">
+      <c r="F92" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20178,7 +20174,7 @@
       <c r="C93" s="21"/>
       <c r="D93" s="220"/>
       <c r="E93" s="130"/>
-      <c r="F93" s="318">
+      <c r="F93" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20198,7 +20194,7 @@
       <c r="C94" s="21"/>
       <c r="D94" s="220"/>
       <c r="E94" s="130"/>
-      <c r="F94" s="318">
+      <c r="F94" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20218,7 +20214,7 @@
       <c r="C95" s="21"/>
       <c r="D95" s="220"/>
       <c r="E95" s="130"/>
-      <c r="F95" s="318">
+      <c r="F95" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20238,7 +20234,7 @@
       <c r="C96" s="21"/>
       <c r="D96" s="220"/>
       <c r="E96" s="130"/>
-      <c r="F96" s="318">
+      <c r="F96" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20258,7 +20254,7 @@
       <c r="C97" s="21"/>
       <c r="D97" s="220"/>
       <c r="E97" s="130"/>
-      <c r="F97" s="318">
+      <c r="F97" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20278,7 +20274,7 @@
       <c r="C98" s="21"/>
       <c r="D98" s="220"/>
       <c r="E98" s="130"/>
-      <c r="F98" s="318">
+      <c r="F98" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20298,7 +20294,7 @@
       <c r="C99" s="21"/>
       <c r="D99" s="220"/>
       <c r="E99" s="130"/>
-      <c r="F99" s="318">
+      <c r="F99" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20318,7 +20314,7 @@
       <c r="C100" s="21"/>
       <c r="D100" s="220"/>
       <c r="E100" s="130"/>
-      <c r="F100" s="318">
+      <c r="F100" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20338,7 +20334,7 @@
       <c r="C101" s="21"/>
       <c r="D101" s="220"/>
       <c r="E101" s="130"/>
-      <c r="F101" s="318">
+      <c r="F101" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20358,7 +20354,7 @@
       <c r="C102" s="21"/>
       <c r="D102" s="220"/>
       <c r="E102" s="130"/>
-      <c r="F102" s="318">
+      <c r="F102" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20378,7 +20374,7 @@
       <c r="C103" s="21"/>
       <c r="D103" s="220"/>
       <c r="E103" s="130"/>
-      <c r="F103" s="318">
+      <c r="F103" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20398,7 +20394,7 @@
       <c r="C104" s="21"/>
       <c r="D104" s="220"/>
       <c r="E104" s="130"/>
-      <c r="F104" s="318">
+      <c r="F104" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20418,7 +20414,7 @@
       <c r="C105" s="21"/>
       <c r="D105" s="220"/>
       <c r="E105" s="130"/>
-      <c r="F105" s="318">
+      <c r="F105" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20438,7 +20434,7 @@
       <c r="C106" s="21"/>
       <c r="D106" s="220"/>
       <c r="E106" s="130"/>
-      <c r="F106" s="318">
+      <c r="F106" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20458,7 +20454,7 @@
       <c r="C107" s="21"/>
       <c r="D107" s="220"/>
       <c r="E107" s="130"/>
-      <c r="F107" s="318">
+      <c r="F107" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20478,7 +20474,7 @@
       <c r="C108" s="21"/>
       <c r="D108" s="220"/>
       <c r="E108" s="130"/>
-      <c r="F108" s="318">
+      <c r="F108" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20498,7 +20494,7 @@
       <c r="C109" s="21"/>
       <c r="D109" s="220"/>
       <c r="E109" s="130"/>
-      <c r="F109" s="318">
+      <c r="F109" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20518,7 +20514,7 @@
       <c r="C110" s="21"/>
       <c r="D110" s="220"/>
       <c r="E110" s="130"/>
-      <c r="F110" s="318">
+      <c r="F110" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20538,7 +20534,7 @@
       <c r="C111" s="21"/>
       <c r="D111" s="220"/>
       <c r="E111" s="130"/>
-      <c r="F111" s="318">
+      <c r="F111" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20558,7 +20554,7 @@
       <c r="C112" s="21"/>
       <c r="D112" s="220"/>
       <c r="E112" s="130"/>
-      <c r="F112" s="318">
+      <c r="F112" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20578,7 +20574,7 @@
       <c r="C113" s="21"/>
       <c r="D113" s="220"/>
       <c r="E113" s="130"/>
-      <c r="F113" s="318">
+      <c r="F113" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20598,7 +20594,7 @@
       <c r="C114" s="21"/>
       <c r="D114" s="220"/>
       <c r="E114" s="130"/>
-      <c r="F114" s="318">
+      <c r="F114" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20618,7 +20614,7 @@
       <c r="C115" s="21"/>
       <c r="D115" s="220"/>
       <c r="E115" s="130"/>
-      <c r="F115" s="318">
+      <c r="F115" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20638,7 +20634,7 @@
       <c r="C116" s="21"/>
       <c r="D116" s="220"/>
       <c r="E116" s="130"/>
-      <c r="F116" s="318">
+      <c r="F116" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20658,7 +20654,7 @@
       <c r="C117" s="21"/>
       <c r="D117" s="220"/>
       <c r="E117" s="130"/>
-      <c r="F117" s="318">
+      <c r="F117" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20678,7 +20674,7 @@
       <c r="C118" s="21"/>
       <c r="D118" s="220"/>
       <c r="E118" s="130"/>
-      <c r="F118" s="318">
+      <c r="F118" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20698,7 +20694,7 @@
       <c r="C119" s="21"/>
       <c r="D119" s="220"/>
       <c r="E119" s="130"/>
-      <c r="F119" s="318">
+      <c r="F119" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20718,7 +20714,7 @@
       <c r="C120" s="21"/>
       <c r="D120" s="220"/>
       <c r="E120" s="130"/>
-      <c r="F120" s="318">
+      <c r="F120" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20738,7 +20734,7 @@
       <c r="C121" s="21"/>
       <c r="D121" s="220"/>
       <c r="E121" s="130"/>
-      <c r="F121" s="318">
+      <c r="F121" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20758,7 +20754,7 @@
       <c r="C122" s="21"/>
       <c r="D122" s="220"/>
       <c r="E122" s="130"/>
-      <c r="F122" s="318">
+      <c r="F122" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20778,7 +20774,7 @@
       <c r="C123" s="21"/>
       <c r="D123" s="220"/>
       <c r="E123" s="130"/>
-      <c r="F123" s="318">
+      <c r="F123" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20798,7 +20794,7 @@
       <c r="C124" s="21"/>
       <c r="D124" s="220"/>
       <c r="E124" s="130"/>
-      <c r="F124" s="318">
+      <c r="F124" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20818,7 +20814,7 @@
       <c r="C125" s="21"/>
       <c r="D125" s="220"/>
       <c r="E125" s="130"/>
-      <c r="F125" s="318">
+      <c r="F125" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20838,7 +20834,7 @@
       <c r="C126" s="21"/>
       <c r="D126" s="220"/>
       <c r="E126" s="130"/>
-      <c r="F126" s="318">
+      <c r="F126" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20858,7 +20854,7 @@
       <c r="C127" s="21"/>
       <c r="D127" s="220"/>
       <c r="E127" s="130"/>
-      <c r="F127" s="318">
+      <c r="F127" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20878,7 +20874,7 @@
       <c r="C128" s="21"/>
       <c r="D128" s="220"/>
       <c r="E128" s="130"/>
-      <c r="F128" s="318">
+      <c r="F128" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20898,7 +20894,7 @@
       <c r="C129" s="21"/>
       <c r="D129" s="220"/>
       <c r="E129" s="130"/>
-      <c r="F129" s="318">
+      <c r="F129" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20918,7 +20914,7 @@
       <c r="C130" s="21"/>
       <c r="D130" s="220"/>
       <c r="E130" s="130"/>
-      <c r="F130" s="318">
+      <c r="F130" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20938,7 +20934,7 @@
       <c r="C131" s="21"/>
       <c r="D131" s="220"/>
       <c r="E131" s="130"/>
-      <c r="F131" s="318">
+      <c r="F131" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20958,7 +20954,7 @@
       <c r="C132" s="21"/>
       <c r="D132" s="220"/>
       <c r="E132" s="130"/>
-      <c r="F132" s="318">
+      <c r="F132" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20978,7 +20974,7 @@
       <c r="C133" s="21"/>
       <c r="D133" s="220"/>
       <c r="E133" s="130"/>
-      <c r="F133" s="318">
+      <c r="F133" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -20998,7 +20994,7 @@
       <c r="C134" s="21"/>
       <c r="D134" s="220"/>
       <c r="E134" s="130"/>
-      <c r="F134" s="318">
+      <c r="F134" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -21018,7 +21014,7 @@
       <c r="C135" s="21"/>
       <c r="D135" s="220"/>
       <c r="E135" s="130"/>
-      <c r="F135" s="318">
+      <c r="F135" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -21038,7 +21034,7 @@
       <c r="C136" s="21"/>
       <c r="D136" s="220"/>
       <c r="E136" s="130"/>
-      <c r="F136" s="318">
+      <c r="F136" s="151">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -21058,7 +21054,7 @@
       <c r="C137" s="21"/>
       <c r="D137" s="220"/>
       <c r="E137" s="130"/>
-      <c r="F137" s="318">
+      <c r="F137" s="151">
         <f t="shared" ref="F137:F179" si="4">SUM(G137,H137)</f>
         <v>0</v>
       </c>
@@ -21078,7 +21074,7 @@
       <c r="C138" s="21"/>
       <c r="D138" s="220"/>
       <c r="E138" s="130"/>
-      <c r="F138" s="318">
+      <c r="F138" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21098,7 +21094,7 @@
       <c r="C139" s="21"/>
       <c r="D139" s="220"/>
       <c r="E139" s="130"/>
-      <c r="F139" s="318">
+      <c r="F139" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21118,7 +21114,7 @@
       <c r="C140" s="21"/>
       <c r="D140" s="220"/>
       <c r="E140" s="130"/>
-      <c r="F140" s="318">
+      <c r="F140" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21138,7 +21134,7 @@
       <c r="C141" s="21"/>
       <c r="D141" s="220"/>
       <c r="E141" s="130"/>
-      <c r="F141" s="318">
+      <c r="F141" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21158,7 +21154,7 @@
       <c r="C142" s="21"/>
       <c r="D142" s="220"/>
       <c r="E142" s="130"/>
-      <c r="F142" s="318">
+      <c r="F142" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21178,7 +21174,7 @@
       <c r="C143" s="21"/>
       <c r="D143" s="220"/>
       <c r="E143" s="130"/>
-      <c r="F143" s="318">
+      <c r="F143" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21198,7 +21194,7 @@
       <c r="C144" s="21"/>
       <c r="D144" s="220"/>
       <c r="E144" s="130"/>
-      <c r="F144" s="318">
+      <c r="F144" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21218,7 +21214,7 @@
       <c r="C145" s="21"/>
       <c r="D145" s="220"/>
       <c r="E145" s="130"/>
-      <c r="F145" s="318">
+      <c r="F145" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21238,7 +21234,7 @@
       <c r="C146" s="21"/>
       <c r="D146" s="220"/>
       <c r="E146" s="130"/>
-      <c r="F146" s="318">
+      <c r="F146" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21258,7 +21254,7 @@
       <c r="C147" s="21"/>
       <c r="D147" s="220"/>
       <c r="E147" s="130"/>
-      <c r="F147" s="318">
+      <c r="F147" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21278,7 +21274,7 @@
       <c r="C148" s="21"/>
       <c r="D148" s="220"/>
       <c r="E148" s="130"/>
-      <c r="F148" s="318">
+      <c r="F148" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21298,7 +21294,7 @@
       <c r="C149" s="21"/>
       <c r="D149" s="220"/>
       <c r="E149" s="130"/>
-      <c r="F149" s="318">
+      <c r="F149" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21318,7 +21314,7 @@
       <c r="C150" s="21"/>
       <c r="D150" s="220"/>
       <c r="E150" s="130"/>
-      <c r="F150" s="318">
+      <c r="F150" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21338,7 +21334,7 @@
       <c r="C151" s="21"/>
       <c r="D151" s="220"/>
       <c r="E151" s="130"/>
-      <c r="F151" s="318">
+      <c r="F151" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21358,7 +21354,7 @@
       <c r="C152" s="21"/>
       <c r="D152" s="220"/>
       <c r="E152" s="130"/>
-      <c r="F152" s="318">
+      <c r="F152" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21378,7 +21374,7 @@
       <c r="C153" s="21"/>
       <c r="D153" s="220"/>
       <c r="E153" s="130"/>
-      <c r="F153" s="318">
+      <c r="F153" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21398,7 +21394,7 @@
       <c r="C154" s="21"/>
       <c r="D154" s="220"/>
       <c r="E154" s="130"/>
-      <c r="F154" s="318">
+      <c r="F154" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21418,7 +21414,7 @@
       <c r="C155" s="21"/>
       <c r="D155" s="220"/>
       <c r="E155" s="130"/>
-      <c r="F155" s="318">
+      <c r="F155" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21438,7 +21434,7 @@
       <c r="C156" s="21"/>
       <c r="D156" s="220"/>
       <c r="E156" s="130"/>
-      <c r="F156" s="318">
+      <c r="F156" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21458,7 +21454,7 @@
       <c r="C157" s="21"/>
       <c r="D157" s="220"/>
       <c r="E157" s="130"/>
-      <c r="F157" s="318">
+      <c r="F157" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21478,7 +21474,7 @@
       <c r="C158" s="21"/>
       <c r="D158" s="220"/>
       <c r="E158" s="130"/>
-      <c r="F158" s="318">
+      <c r="F158" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21498,7 +21494,7 @@
       <c r="C159" s="21"/>
       <c r="D159" s="220"/>
       <c r="E159" s="130"/>
-      <c r="F159" s="318">
+      <c r="F159" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21518,7 +21514,7 @@
       <c r="C160" s="21"/>
       <c r="D160" s="220"/>
       <c r="E160" s="130"/>
-      <c r="F160" s="318">
+      <c r="F160" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21538,7 +21534,7 @@
       <c r="C161" s="21"/>
       <c r="D161" s="220"/>
       <c r="E161" s="130"/>
-      <c r="F161" s="318">
+      <c r="F161" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21558,7 +21554,7 @@
       <c r="C162" s="21"/>
       <c r="D162" s="220"/>
       <c r="E162" s="130"/>
-      <c r="F162" s="318">
+      <c r="F162" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21578,7 +21574,7 @@
       <c r="C163" s="21"/>
       <c r="D163" s="220"/>
       <c r="E163" s="130"/>
-      <c r="F163" s="318">
+      <c r="F163" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21598,7 +21594,7 @@
       <c r="C164" s="21"/>
       <c r="D164" s="220"/>
       <c r="E164" s="130"/>
-      <c r="F164" s="318">
+      <c r="F164" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21618,7 +21614,7 @@
       <c r="C165" s="21"/>
       <c r="D165" s="220"/>
       <c r="E165" s="130"/>
-      <c r="F165" s="318">
+      <c r="F165" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21638,7 +21634,7 @@
       <c r="C166" s="21"/>
       <c r="D166" s="220"/>
       <c r="E166" s="130"/>
-      <c r="F166" s="318">
+      <c r="F166" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21658,7 +21654,7 @@
       <c r="C167" s="21"/>
       <c r="D167" s="220"/>
       <c r="E167" s="130"/>
-      <c r="F167" s="318">
+      <c r="F167" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21678,7 +21674,7 @@
       <c r="C168" s="21"/>
       <c r="D168" s="220"/>
       <c r="E168" s="130"/>
-      <c r="F168" s="318">
+      <c r="F168" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21698,7 +21694,7 @@
       <c r="C169" s="21"/>
       <c r="D169" s="220"/>
       <c r="E169" s="130"/>
-      <c r="F169" s="318">
+      <c r="F169" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21718,7 +21714,7 @@
       <c r="C170" s="21"/>
       <c r="D170" s="220"/>
       <c r="E170" s="130"/>
-      <c r="F170" s="318">
+      <c r="F170" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21738,7 +21734,7 @@
       <c r="C171" s="21"/>
       <c r="D171" s="220"/>
       <c r="E171" s="130"/>
-      <c r="F171" s="318">
+      <c r="F171" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21758,7 +21754,7 @@
       <c r="C172" s="21"/>
       <c r="D172" s="220"/>
       <c r="E172" s="130"/>
-      <c r="F172" s="318">
+      <c r="F172" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21778,7 +21774,7 @@
       <c r="C173" s="21"/>
       <c r="D173" s="220"/>
       <c r="E173" s="130"/>
-      <c r="F173" s="318">
+      <c r="F173" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21798,7 +21794,7 @@
       <c r="C174" s="21"/>
       <c r="D174" s="220"/>
       <c r="E174" s="130"/>
-      <c r="F174" s="318">
+      <c r="F174" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21818,7 +21814,7 @@
       <c r="C175" s="21"/>
       <c r="D175" s="220"/>
       <c r="E175" s="130"/>
-      <c r="F175" s="318">
+      <c r="F175" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21838,7 +21834,7 @@
       <c r="C176" s="21"/>
       <c r="D176" s="220"/>
       <c r="E176" s="130"/>
-      <c r="F176" s="318">
+      <c r="F176" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21858,7 +21854,7 @@
       <c r="C177" s="21"/>
       <c r="D177" s="220"/>
       <c r="E177" s="130"/>
-      <c r="F177" s="318">
+      <c r="F177" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21878,7 +21874,7 @@
       <c r="C178" s="21"/>
       <c r="D178" s="220"/>
       <c r="E178" s="130"/>
-      <c r="F178" s="318">
+      <c r="F178" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21898,7 +21894,7 @@
       <c r="C179" s="219"/>
       <c r="D179" s="232"/>
       <c r="E179" s="225"/>
-      <c r="F179" s="318">
+      <c r="F179" s="151">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -21913,7 +21909,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" ht="18" customHeight="1">
-      <c r="A180" s="305" t="s">
+      <c r="A180" s="304" t="s">
         <v>386</v>
       </c>
       <c r="B180" s="274"/>
@@ -22080,7 +22076,7 @@
         <v>0</v>
       </c>
       <c r="J186" s="271"/>
-      <c r="K186" s="304"/>
+      <c r="K186" s="307"/>
       <c r="L186" s="300"/>
     </row>
     <row r="187" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22111,7 +22107,7 @@
         <v>0</v>
       </c>
       <c r="J187" s="271"/>
-      <c r="K187" s="304"/>
+      <c r="K187" s="307"/>
       <c r="L187" s="300"/>
     </row>
     <row r="188" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22142,7 +22138,7 @@
         <v>0</v>
       </c>
       <c r="J188" s="271"/>
-      <c r="K188" s="304"/>
+      <c r="K188" s="307"/>
       <c r="L188" s="300"/>
     </row>
     <row r="189" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22173,7 +22169,7 @@
         <v>0</v>
       </c>
       <c r="J189" s="271"/>
-      <c r="K189" s="304"/>
+      <c r="K189" s="307"/>
       <c r="L189" s="300"/>
     </row>
     <row r="190" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22204,7 +22200,7 @@
         <v>0</v>
       </c>
       <c r="J190" s="271"/>
-      <c r="K190" s="304"/>
+      <c r="K190" s="307"/>
       <c r="L190" s="300"/>
     </row>
     <row r="191" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22235,7 +22231,7 @@
         <v>0</v>
       </c>
       <c r="J191" s="271"/>
-      <c r="K191" s="304"/>
+      <c r="K191" s="307"/>
       <c r="L191" s="300"/>
     </row>
     <row r="192" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22266,7 +22262,7 @@
         <v>0</v>
       </c>
       <c r="J192" s="271"/>
-      <c r="K192" s="304"/>
+      <c r="K192" s="307"/>
       <c r="L192" s="300"/>
     </row>
     <row r="193" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22297,7 +22293,7 @@
         <v>0</v>
       </c>
       <c r="J193" s="271"/>
-      <c r="K193" s="304"/>
+      <c r="K193" s="307"/>
       <c r="L193" s="300"/>
     </row>
     <row r="194" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22328,7 +22324,7 @@
         <v>0</v>
       </c>
       <c r="J194" s="271"/>
-      <c r="K194" s="304"/>
+      <c r="K194" s="307"/>
       <c r="L194" s="300"/>
     </row>
     <row r="195" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22359,7 +22355,7 @@
         <v>0</v>
       </c>
       <c r="J195" s="271"/>
-      <c r="K195" s="304"/>
+      <c r="K195" s="307"/>
       <c r="L195" s="300"/>
     </row>
     <row r="196" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22390,7 +22386,7 @@
         <v>0</v>
       </c>
       <c r="J196" s="271"/>
-      <c r="K196" s="304"/>
+      <c r="K196" s="307"/>
       <c r="L196" s="300"/>
     </row>
     <row r="197" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22421,7 +22417,7 @@
         <v>0</v>
       </c>
       <c r="J197" s="271"/>
-      <c r="K197" s="304"/>
+      <c r="K197" s="307"/>
       <c r="L197" s="300"/>
     </row>
     <row r="198" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
@@ -22452,7 +22448,7 @@
         <v>0</v>
       </c>
       <c r="J198" s="279"/>
-      <c r="K198" s="307"/>
+      <c r="K198" s="306"/>
       <c r="L198" s="295"/>
     </row>
     <row r="199" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
@@ -22571,12 +22567,12 @@
       <c r="B205" s="301"/>
       <c r="C205" s="300"/>
       <c r="D205" s="311"/>
-      <c r="E205" s="304"/>
-      <c r="F205" s="304"/>
-      <c r="G205" s="304"/>
-      <c r="H205" s="304"/>
-      <c r="I205" s="304"/>
-      <c r="J205" s="304"/>
+      <c r="E205" s="307"/>
+      <c r="F205" s="307"/>
+      <c r="G205" s="307"/>
+      <c r="H205" s="307"/>
+      <c r="I205" s="307"/>
+      <c r="J205" s="307"/>
       <c r="K205" s="300"/>
       <c r="L205" s="121"/>
     </row>
@@ -22587,12 +22583,12 @@
       <c r="B206" s="301"/>
       <c r="C206" s="300"/>
       <c r="D206" s="309"/>
-      <c r="E206" s="304"/>
-      <c r="F206" s="304"/>
-      <c r="G206" s="304"/>
-      <c r="H206" s="304"/>
-      <c r="I206" s="304"/>
-      <c r="J206" s="304"/>
+      <c r="E206" s="307"/>
+      <c r="F206" s="307"/>
+      <c r="G206" s="307"/>
+      <c r="H206" s="307"/>
+      <c r="I206" s="307"/>
+      <c r="J206" s="307"/>
       <c r="K206" s="300"/>
       <c r="L206" s="122"/>
     </row>
@@ -22603,12 +22599,12 @@
       <c r="B207" s="301"/>
       <c r="C207" s="300"/>
       <c r="D207" s="311"/>
-      <c r="E207" s="304"/>
-      <c r="F207" s="304"/>
-      <c r="G207" s="304"/>
-      <c r="H207" s="304"/>
-      <c r="I207" s="304"/>
-      <c r="J207" s="304"/>
+      <c r="E207" s="307"/>
+      <c r="F207" s="307"/>
+      <c r="G207" s="307"/>
+      <c r="H207" s="307"/>
+      <c r="I207" s="307"/>
+      <c r="J207" s="307"/>
       <c r="K207" s="300"/>
       <c r="L207" s="121"/>
     </row>
@@ -22618,13 +22614,13 @@
       </c>
       <c r="B208" s="314"/>
       <c r="C208" s="295"/>
-      <c r="D208" s="306"/>
-      <c r="E208" s="307"/>
-      <c r="F208" s="307"/>
-      <c r="G208" s="307"/>
-      <c r="H208" s="307"/>
-      <c r="I208" s="307"/>
-      <c r="J208" s="307"/>
+      <c r="D208" s="305"/>
+      <c r="E208" s="306"/>
+      <c r="F208" s="306"/>
+      <c r="G208" s="306"/>
+      <c r="H208" s="306"/>
+      <c r="I208" s="306"/>
+      <c r="J208" s="306"/>
       <c r="K208" s="295"/>
       <c r="L208" s="123"/>
     </row>
@@ -22651,12 +22647,12 @@
       <c r="B210" s="299"/>
       <c r="C210" s="300"/>
       <c r="D210" s="311"/>
-      <c r="E210" s="304"/>
-      <c r="F210" s="304"/>
-      <c r="G210" s="304"/>
-      <c r="H210" s="304"/>
-      <c r="I210" s="304"/>
-      <c r="J210" s="304"/>
+      <c r="E210" s="307"/>
+      <c r="F210" s="307"/>
+      <c r="G210" s="307"/>
+      <c r="H210" s="307"/>
+      <c r="I210" s="307"/>
+      <c r="J210" s="307"/>
       <c r="K210" s="300"/>
       <c r="L210" s="121"/>
     </row>
@@ -22667,12 +22663,12 @@
       <c r="B211" s="299"/>
       <c r="C211" s="300"/>
       <c r="D211" s="311"/>
-      <c r="E211" s="304"/>
-      <c r="F211" s="304"/>
-      <c r="G211" s="304"/>
-      <c r="H211" s="304"/>
-      <c r="I211" s="304"/>
-      <c r="J211" s="304"/>
+      <c r="E211" s="307"/>
+      <c r="F211" s="307"/>
+      <c r="G211" s="307"/>
+      <c r="H211" s="307"/>
+      <c r="I211" s="307"/>
+      <c r="J211" s="307"/>
       <c r="K211" s="300"/>
       <c r="L211" s="121"/>
     </row>
@@ -22683,12 +22679,12 @@
       <c r="B212" s="299"/>
       <c r="C212" s="300"/>
       <c r="D212" s="311"/>
-      <c r="E212" s="304"/>
-      <c r="F212" s="304"/>
-      <c r="G212" s="304"/>
-      <c r="H212" s="304"/>
-      <c r="I212" s="304"/>
-      <c r="J212" s="304"/>
+      <c r="E212" s="307"/>
+      <c r="F212" s="307"/>
+      <c r="G212" s="307"/>
+      <c r="H212" s="307"/>
+      <c r="I212" s="307"/>
+      <c r="J212" s="307"/>
       <c r="K212" s="300"/>
       <c r="L212" s="121"/>
     </row>
@@ -22698,13 +22694,13 @@
       </c>
       <c r="B213" s="294"/>
       <c r="C213" s="295"/>
-      <c r="D213" s="306"/>
-      <c r="E213" s="307"/>
-      <c r="F213" s="307"/>
-      <c r="G213" s="307"/>
-      <c r="H213" s="307"/>
-      <c r="I213" s="307"/>
-      <c r="J213" s="307"/>
+      <c r="D213" s="305"/>
+      <c r="E213" s="306"/>
+      <c r="F213" s="306"/>
+      <c r="G213" s="306"/>
+      <c r="H213" s="306"/>
+      <c r="I213" s="306"/>
+      <c r="J213" s="306"/>
       <c r="K213" s="295"/>
       <c r="L213" s="123"/>
     </row>
@@ -22801,12 +22797,12 @@
       <c r="B219" s="301"/>
       <c r="C219" s="300"/>
       <c r="D219" s="311"/>
-      <c r="E219" s="304"/>
-      <c r="F219" s="304"/>
-      <c r="G219" s="304"/>
-      <c r="H219" s="304"/>
-      <c r="I219" s="304"/>
-      <c r="J219" s="304"/>
+      <c r="E219" s="307"/>
+      <c r="F219" s="307"/>
+      <c r="G219" s="307"/>
+      <c r="H219" s="307"/>
+      <c r="I219" s="307"/>
+      <c r="J219" s="307"/>
       <c r="K219" s="300"/>
       <c r="L219" s="121"/>
     </row>
@@ -22817,12 +22813,12 @@
       <c r="B220" s="301"/>
       <c r="C220" s="300"/>
       <c r="D220" s="309"/>
-      <c r="E220" s="304"/>
-      <c r="F220" s="304"/>
-      <c r="G220" s="304"/>
-      <c r="H220" s="304"/>
-      <c r="I220" s="304"/>
-      <c r="J220" s="304"/>
+      <c r="E220" s="307"/>
+      <c r="F220" s="307"/>
+      <c r="G220" s="307"/>
+      <c r="H220" s="307"/>
+      <c r="I220" s="307"/>
+      <c r="J220" s="307"/>
       <c r="K220" s="300"/>
       <c r="L220" s="122"/>
     </row>
@@ -22833,12 +22829,12 @@
       <c r="B221" s="301"/>
       <c r="C221" s="300"/>
       <c r="D221" s="311"/>
-      <c r="E221" s="304"/>
-      <c r="F221" s="304"/>
-      <c r="G221" s="304"/>
-      <c r="H221" s="304"/>
-      <c r="I221" s="304"/>
-      <c r="J221" s="304"/>
+      <c r="E221" s="307"/>
+      <c r="F221" s="307"/>
+      <c r="G221" s="307"/>
+      <c r="H221" s="307"/>
+      <c r="I221" s="307"/>
+      <c r="J221" s="307"/>
       <c r="K221" s="300"/>
       <c r="L221" s="121"/>
     </row>
@@ -22849,12 +22845,12 @@
       <c r="B222" s="301"/>
       <c r="C222" s="300"/>
       <c r="D222" s="311"/>
-      <c r="E222" s="304"/>
-      <c r="F222" s="304"/>
-      <c r="G222" s="304"/>
-      <c r="H222" s="304"/>
-      <c r="I222" s="304"/>
-      <c r="J222" s="304"/>
+      <c r="E222" s="307"/>
+      <c r="F222" s="307"/>
+      <c r="G222" s="307"/>
+      <c r="H222" s="307"/>
+      <c r="I222" s="307"/>
+      <c r="J222" s="307"/>
       <c r="K222" s="300"/>
       <c r="L222" s="121"/>
     </row>
@@ -22865,12 +22861,12 @@
       <c r="B223" s="299"/>
       <c r="C223" s="300"/>
       <c r="D223" s="311"/>
-      <c r="E223" s="304"/>
-      <c r="F223" s="304"/>
-      <c r="G223" s="304"/>
-      <c r="H223" s="304"/>
-      <c r="I223" s="304"/>
-      <c r="J223" s="304"/>
+      <c r="E223" s="307"/>
+      <c r="F223" s="307"/>
+      <c r="G223" s="307"/>
+      <c r="H223" s="307"/>
+      <c r="I223" s="307"/>
+      <c r="J223" s="307"/>
       <c r="K223" s="300"/>
       <c r="L223" s="121"/>
     </row>
@@ -22881,12 +22877,12 @@
       <c r="B224" s="299"/>
       <c r="C224" s="300"/>
       <c r="D224" s="311"/>
-      <c r="E224" s="304"/>
-      <c r="F224" s="304"/>
-      <c r="G224" s="304"/>
-      <c r="H224" s="304"/>
-      <c r="I224" s="304"/>
-      <c r="J224" s="304"/>
+      <c r="E224" s="307"/>
+      <c r="F224" s="307"/>
+      <c r="G224" s="307"/>
+      <c r="H224" s="307"/>
+      <c r="I224" s="307"/>
+      <c r="J224" s="307"/>
       <c r="K224" s="300"/>
       <c r="L224" s="121"/>
     </row>
@@ -22897,12 +22893,12 @@
       <c r="B225" s="299"/>
       <c r="C225" s="300"/>
       <c r="D225" s="311"/>
-      <c r="E225" s="304"/>
-      <c r="F225" s="304"/>
-      <c r="G225" s="304"/>
-      <c r="H225" s="304"/>
-      <c r="I225" s="304"/>
-      <c r="J225" s="304"/>
+      <c r="E225" s="307"/>
+      <c r="F225" s="307"/>
+      <c r="G225" s="307"/>
+      <c r="H225" s="307"/>
+      <c r="I225" s="307"/>
+      <c r="J225" s="307"/>
       <c r="K225" s="300"/>
       <c r="L225" s="121"/>
     </row>
@@ -22913,12 +22909,12 @@
       <c r="B226" s="299"/>
       <c r="C226" s="300"/>
       <c r="D226" s="311"/>
-      <c r="E226" s="304"/>
-      <c r="F226" s="304"/>
-      <c r="G226" s="304"/>
-      <c r="H226" s="304"/>
-      <c r="I226" s="304"/>
-      <c r="J226" s="304"/>
+      <c r="E226" s="307"/>
+      <c r="F226" s="307"/>
+      <c r="G226" s="307"/>
+      <c r="H226" s="307"/>
+      <c r="I226" s="307"/>
+      <c r="J226" s="307"/>
       <c r="K226" s="300"/>
       <c r="L226" s="121"/>
     </row>
@@ -22928,13 +22924,13 @@
       </c>
       <c r="B227" s="294"/>
       <c r="C227" s="295"/>
-      <c r="D227" s="306"/>
-      <c r="E227" s="307"/>
-      <c r="F227" s="307"/>
-      <c r="G227" s="307"/>
-      <c r="H227" s="307"/>
-      <c r="I227" s="307"/>
-      <c r="J227" s="307"/>
+      <c r="D227" s="305"/>
+      <c r="E227" s="306"/>
+      <c r="F227" s="306"/>
+      <c r="G227" s="306"/>
+      <c r="H227" s="306"/>
+      <c r="I227" s="306"/>
+      <c r="J227" s="306"/>
       <c r="K227" s="295"/>
       <c r="L227" s="123"/>
     </row>
@@ -23230,8 +23226,6 @@
     <mergeCell ref="B208:C208"/>
     <mergeCell ref="D222:K222"/>
     <mergeCell ref="B224:C224"/>
-    <mergeCell ref="J185:L185"/>
-    <mergeCell ref="D227:K227"/>
     <mergeCell ref="J188:L188"/>
     <mergeCell ref="J194:L194"/>
     <mergeCell ref="D212:K212"/>
@@ -23241,10 +23235,8 @@
     <mergeCell ref="D219:K219"/>
     <mergeCell ref="D213:K213"/>
     <mergeCell ref="A215:L215"/>
-    <mergeCell ref="D225:K225"/>
     <mergeCell ref="D210:K210"/>
     <mergeCell ref="A214:K214"/>
-    <mergeCell ref="B226:C226"/>
     <mergeCell ref="J197:L197"/>
     <mergeCell ref="A180:D180"/>
     <mergeCell ref="D203:K203"/>
@@ -23261,6 +23253,7 @@
     <mergeCell ref="J198:L198"/>
     <mergeCell ref="B205:C205"/>
     <mergeCell ref="J189:L189"/>
+    <mergeCell ref="J185:L185"/>
     <mergeCell ref="B218:C218"/>
     <mergeCell ref="B209:C209"/>
     <mergeCell ref="B227:C227"/>
@@ -23269,6 +23262,9 @@
     <mergeCell ref="B223:C223"/>
     <mergeCell ref="B220:C220"/>
     <mergeCell ref="D209:K209"/>
+    <mergeCell ref="D227:K227"/>
+    <mergeCell ref="D225:K225"/>
+    <mergeCell ref="B226:C226"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0300-000000000000}">

</xml_diff>

<commit_message>
Update mau_kegio.xlsx to reflect recent data modifications and enhance overall formatting
</commit_message>
<xml_diff>
--- a/data_base/mau_kegio.xlsx
+++ b/data_base/mau_kegio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0E07FD-7CBC-4A74-9994-0E29EA0CE5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E721910-098E-4996-903A-1A9A4406A619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hướng dẫn" sheetId="1" r:id="rId1"/>
@@ -2323,7 +2323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2643,6 +2643,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2664,7 +2690,7 @@
     <xf numFmtId="172" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="321">
+  <cellXfs count="327">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3490,6 +3516,22 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3528,39 +3570,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -3589,10 +3617,34 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
@@ -3601,116 +3653,114 @@
       <alignment shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -4561,25 +4611,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="16.899999999999999" customHeight="1">
-      <c r="A2" s="250" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="251"/>
-      <c r="C2" s="251"/>
-      <c r="D2" s="251"/>
-      <c r="E2" s="251"/>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
-      <c r="L2" s="251"/>
-      <c r="M2" s="251"/>
-      <c r="N2" s="251"/>
-      <c r="O2" s="251"/>
-      <c r="P2" s="251"/>
-      <c r="Q2" s="251"/>
+      <c r="A2" s="254" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="255"/>
+      <c r="C2" s="255"/>
+      <c r="D2" s="255"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="255"/>
+      <c r="G2" s="255"/>
+      <c r="H2" s="255"/>
+      <c r="I2" s="255"/>
+      <c r="J2" s="255"/>
+      <c r="K2" s="255"/>
+      <c r="L2" s="255"/>
+      <c r="M2" s="255"/>
+      <c r="N2" s="255"/>
+      <c r="O2" s="255"/>
+      <c r="P2" s="255"/>
+      <c r="Q2" s="255"/>
     </row>
     <row r="3" spans="1:17" s="3" customFormat="1" ht="17.45" customHeight="1">
       <c r="A3" s="6"/>
@@ -4770,18 +4820,18 @@
     </row>
     <row r="22" spans="1:256" s="191" customFormat="1" ht="18" customHeight="1">
       <c r="B22" s="192"/>
-      <c r="C22" s="256" t="s">
+      <c r="C22" s="260" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="257"/>
-      <c r="E22" s="257"/>
-      <c r="F22" s="257"/>
-      <c r="G22" s="257"/>
-      <c r="H22" s="257"/>
-      <c r="I22" s="257"/>
-      <c r="J22" s="257"/>
-      <c r="K22" s="257"/>
-      <c r="L22" s="257"/>
+      <c r="D22" s="261"/>
+      <c r="E22" s="261"/>
+      <c r="F22" s="261"/>
+      <c r="G22" s="261"/>
+      <c r="H22" s="261"/>
+      <c r="I22" s="261"/>
+      <c r="J22" s="261"/>
+      <c r="K22" s="261"/>
+      <c r="L22" s="261"/>
     </row>
     <row r="23" spans="1:256" ht="21" customHeight="1">
       <c r="A23" s="5">
@@ -5761,18 +5811,18 @@
       <c r="C54" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="254" t="s">
+      <c r="D54" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="255"/>
-      <c r="F54" s="254" t="s">
+      <c r="E54" s="259"/>
+      <c r="F54" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="255"/>
-      <c r="H54" s="254" t="s">
+      <c r="G54" s="259"/>
+      <c r="H54" s="258" t="s">
         <v>24</v>
       </c>
-      <c r="I54" s="255"/>
+      <c r="I54" s="259"/>
       <c r="J54" s="138" t="s">
         <v>25</v>
       </c>
@@ -5959,18 +6009,18 @@
       <c r="C62" s="140">
         <v>7</v>
       </c>
-      <c r="D62" s="252" t="s">
+      <c r="D62" s="256" t="s">
         <v>29</v>
       </c>
-      <c r="E62" s="253"/>
-      <c r="F62" s="252" t="s">
+      <c r="E62" s="257"/>
+      <c r="F62" s="256" t="s">
         <v>30</v>
       </c>
-      <c r="G62" s="253"/>
-      <c r="H62" s="252" t="s">
+      <c r="G62" s="257"/>
+      <c r="H62" s="256" t="s">
         <v>31</v>
       </c>
-      <c r="I62" s="253"/>
+      <c r="I62" s="257"/>
       <c r="J62" s="143">
         <v>1.3</v>
       </c>
@@ -6158,36 +6208,36 @@
       <c r="R1" s="96"/>
     </row>
     <row r="2" spans="1:19" ht="21" customHeight="1">
-      <c r="A2" s="261" t="s">
+      <c r="A2" s="265" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="262"/>
-      <c r="C2" s="262"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="264"/>
-      <c r="H2" s="264"/>
-      <c r="I2" s="264"/>
-      <c r="J2" s="264"/>
-      <c r="K2" s="264"/>
-      <c r="L2" s="264"/>
-      <c r="M2" s="264"/>
-      <c r="N2" s="264"/>
-      <c r="O2" s="264"/>
-      <c r="P2" s="264"/>
-      <c r="Q2" s="264"/>
-      <c r="R2" s="264"/>
-      <c r="S2" s="264"/>
+      <c r="B2" s="266"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="267"/>
+      <c r="F2" s="267"/>
+      <c r="G2" s="268"/>
+      <c r="H2" s="268"/>
+      <c r="I2" s="268"/>
+      <c r="J2" s="268"/>
+      <c r="K2" s="268"/>
+      <c r="L2" s="268"/>
+      <c r="M2" s="268"/>
+      <c r="N2" s="268"/>
+      <c r="O2" s="268"/>
+      <c r="P2" s="268"/>
+      <c r="Q2" s="268"/>
+      <c r="R2" s="268"/>
+      <c r="S2" s="268"/>
     </row>
     <row r="4" spans="1:19" ht="21" customHeight="1">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="269" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="266"/>
-      <c r="D4" s="266"/>
-      <c r="E4" s="255"/>
+      <c r="B4" s="270"/>
+      <c r="C4" s="270"/>
+      <c r="D4" s="270"/>
+      <c r="E4" s="259"/>
       <c r="F4" s="104" t="s">
         <v>52</v>
       </c>
@@ -6227,16 +6277,16 @@
       <c r="R4" s="132" t="s">
         <v>64</v>
       </c>
-      <c r="S4" s="258" t="s">
+      <c r="S4" s="262" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="37.15" customHeight="1">
-      <c r="A5" s="267"/>
-      <c r="B5" s="268"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="269"/>
+      <c r="A5" s="271"/>
+      <c r="B5" s="272"/>
+      <c r="C5" s="272"/>
+      <c r="D5" s="272"/>
+      <c r="E5" s="273"/>
       <c r="F5" s="137" t="s">
         <v>66</v>
       </c>
@@ -6276,7 +6326,7 @@
       <c r="R5" s="132" t="s">
         <v>78</v>
       </c>
-      <c r="S5" s="259"/>
+      <c r="S5" s="263"/>
     </row>
     <row r="6" spans="1:19" s="39" customFormat="1" ht="21.6" customHeight="1">
       <c r="A6" s="103" t="s">
@@ -6329,7 +6379,7 @@
       <c r="R6" s="133">
         <v>45839</v>
       </c>
-      <c r="S6" s="260"/>
+      <c r="S6" s="264"/>
     </row>
     <row r="7" spans="1:19" ht="18" customHeight="1">
       <c r="A7" s="40" t="s">
@@ -13949,8 +13999,8 @@
   </sheetPr>
   <dimension ref="A1:N211"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" topLeftCell="A181" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185:D202"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A180" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F203" sqref="F203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -13978,14 +14028,14 @@
       <c r="D1" s="280" t="s">
         <v>364</v>
       </c>
-      <c r="E1" s="276"/>
-      <c r="F1" s="276"/>
-      <c r="G1" s="276"/>
-      <c r="H1" s="276"/>
-      <c r="I1" s="276"/>
-      <c r="J1" s="276"/>
-      <c r="K1" s="276"/>
-      <c r="L1" s="276"/>
+      <c r="E1" s="275"/>
+      <c r="F1" s="275"/>
+      <c r="G1" s="275"/>
+      <c r="H1" s="275"/>
+      <c r="I1" s="275"/>
+      <c r="J1" s="275"/>
+      <c r="K1" s="275"/>
+      <c r="L1" s="275"/>
     </row>
     <row r="2" spans="1:12">
       <c r="B2" s="11"/>
@@ -14019,9 +14069,9 @@
         <v>369</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
+      <c r="J4" s="292"/>
+      <c r="K4" s="275"/>
+      <c r="L4" s="275"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="10" t="s">
@@ -17540,12 +17590,12 @@
       </c>
     </row>
     <row r="180" spans="1:14" ht="16.5" customHeight="1">
-      <c r="A180" s="272" t="s">
+      <c r="A180" s="291" t="s">
         <v>386</v>
       </c>
-      <c r="B180" s="273"/>
-      <c r="C180" s="273"/>
-      <c r="D180" s="274"/>
+      <c r="B180" s="288"/>
+      <c r="C180" s="288"/>
+      <c r="D180" s="289"/>
       <c r="E180" s="80"/>
       <c r="F180" s="165">
         <f>SUM(F8:F179)</f>
@@ -17588,17 +17638,17 @@
       <c r="A182" s="281" t="s">
         <v>387</v>
       </c>
-      <c r="B182" s="276"/>
-      <c r="C182" s="276"/>
-      <c r="D182" s="276"/>
-      <c r="E182" s="276"/>
-      <c r="F182" s="276"/>
-      <c r="G182" s="276"/>
-      <c r="H182" s="276"/>
-      <c r="I182" s="276"/>
-      <c r="J182" s="276"/>
-      <c r="K182" s="276"/>
-      <c r="L182" s="276"/>
+      <c r="B182" s="275"/>
+      <c r="C182" s="275"/>
+      <c r="D182" s="275"/>
+      <c r="E182" s="275"/>
+      <c r="F182" s="275"/>
+      <c r="G182" s="275"/>
+      <c r="H182" s="275"/>
+      <c r="I182" s="275"/>
+      <c r="J182" s="275"/>
+      <c r="K182" s="275"/>
+      <c r="L182" s="275"/>
     </row>
     <row r="183" spans="1:14" s="20" customFormat="1" ht="12.95" customHeight="1">
       <c r="A183" s="232"/>
@@ -17654,7 +17704,7 @@
       </c>
       <c r="B185" s="88"/>
       <c r="C185" s="88"/>
-      <c r="D185" s="320"/>
+      <c r="D185" s="253"/>
       <c r="E185" s="154">
         <f t="array" ref="E185">MIN(IF(($B$8:$B$180=B185)*($D$8:$D$180=D185), $E$8:$E$180))</f>
         <v>0</v>
@@ -17671,10 +17721,13 @@
         <f t="shared" ref="H185:H202" si="14">SUMIFS($H$8:$H$180, $B$8:$B$180,B185,$D$8:$D$180,D185)</f>
         <v>0</v>
       </c>
-      <c r="I185" s="176"/>
-      <c r="J185" s="270"/>
-      <c r="K185" s="271"/>
-      <c r="L185" s="271"/>
+      <c r="I185" s="155">
+        <f t="shared" ref="I185:I202" si="15">SUMIFS($L$8:$L$180, $B$8:$B$180,B185,$D$8:$D$180,D185)</f>
+        <v>0</v>
+      </c>
+      <c r="J185" s="278"/>
+      <c r="K185" s="279"/>
+      <c r="L185" s="279"/>
     </row>
     <row r="186" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A186" s="226">
@@ -17682,7 +17735,7 @@
       </c>
       <c r="B186" s="88"/>
       <c r="C186" s="88"/>
-      <c r="D186" s="318"/>
+      <c r="D186" s="251"/>
       <c r="E186" s="154">
         <f t="array" ref="E186">MIN(IF(($B$8:$B$180=B186)*($D$8:$D$180=D186), $E$8:$E$180))</f>
         <v>0</v>
@@ -17700,12 +17753,12 @@
         <v>0</v>
       </c>
       <c r="I186" s="155">
-        <f t="shared" ref="I186:I202" si="15">SUMIFS($L$8:$L$180, $B$8:$B$180,B186,$D$8:$D$180,D186)</f>
-        <v>0</v>
-      </c>
-      <c r="J186" s="270"/>
-      <c r="K186" s="271"/>
-      <c r="L186" s="271"/>
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="J186" s="278"/>
+      <c r="K186" s="279"/>
+      <c r="L186" s="279"/>
     </row>
     <row r="187" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A187" s="226">
@@ -17713,7 +17766,7 @@
       </c>
       <c r="B187" s="88"/>
       <c r="C187" s="88"/>
-      <c r="D187" s="318"/>
+      <c r="D187" s="251"/>
       <c r="E187" s="154">
         <f t="array" ref="E187">MIN(IF(($B$8:$B$180=B187)*($D$8:$D$180=D187), $E$8:$E$180))</f>
         <v>0</v>
@@ -17734,9 +17787,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J187" s="270"/>
-      <c r="K187" s="271"/>
-      <c r="L187" s="271"/>
+      <c r="J187" s="278"/>
+      <c r="K187" s="279"/>
+      <c r="L187" s="279"/>
     </row>
     <row r="188" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A188" s="226">
@@ -17744,7 +17797,7 @@
       </c>
       <c r="B188" s="88"/>
       <c r="C188" s="88"/>
-      <c r="D188" s="318"/>
+      <c r="D188" s="251"/>
       <c r="E188" s="154">
         <f t="array" ref="E188">MIN(IF(($B$8:$B$180=B188)*($D$8:$D$180=D188), $E$8:$E$180))</f>
         <v>0</v>
@@ -17765,9 +17818,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J188" s="270"/>
-      <c r="K188" s="271"/>
-      <c r="L188" s="271"/>
+      <c r="J188" s="278"/>
+      <c r="K188" s="279"/>
+      <c r="L188" s="279"/>
     </row>
     <row r="189" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A189" s="226">
@@ -17775,7 +17828,7 @@
       </c>
       <c r="B189" s="88"/>
       <c r="C189" s="88"/>
-      <c r="D189" s="318"/>
+      <c r="D189" s="251"/>
       <c r="E189" s="154">
         <f t="array" ref="E189">MIN(IF(($B$8:$B$180=B189)*($D$8:$D$180=D189), $E$8:$E$180))</f>
         <v>0</v>
@@ -17796,9 +17849,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J189" s="270"/>
-      <c r="K189" s="271"/>
-      <c r="L189" s="271"/>
+      <c r="J189" s="278"/>
+      <c r="K189" s="279"/>
+      <c r="L189" s="279"/>
     </row>
     <row r="190" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A190" s="226">
@@ -17806,7 +17859,7 @@
       </c>
       <c r="B190" s="88"/>
       <c r="C190" s="88"/>
-      <c r="D190" s="318"/>
+      <c r="D190" s="251"/>
       <c r="E190" s="154">
         <f t="array" ref="E190">MIN(IF(($B$8:$B$180=B190)*($D$8:$D$180=D190), $E$8:$E$180))</f>
         <v>0</v>
@@ -17827,9 +17880,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J190" s="270"/>
-      <c r="K190" s="271"/>
-      <c r="L190" s="271"/>
+      <c r="J190" s="278"/>
+      <c r="K190" s="279"/>
+      <c r="L190" s="279"/>
     </row>
     <row r="191" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A191" s="226">
@@ -17837,7 +17890,7 @@
       </c>
       <c r="B191" s="88"/>
       <c r="C191" s="88"/>
-      <c r="D191" s="318"/>
+      <c r="D191" s="251"/>
       <c r="E191" s="154">
         <f t="array" ref="E191">MIN(IF(($B$8:$B$180=B191)*($D$8:$D$180=D191), $E$8:$E$180))</f>
         <v>0</v>
@@ -17858,9 +17911,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J191" s="270"/>
-      <c r="K191" s="271"/>
-      <c r="L191" s="271"/>
+      <c r="J191" s="278"/>
+      <c r="K191" s="279"/>
+      <c r="L191" s="279"/>
     </row>
     <row r="192" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A192" s="226">
@@ -17868,7 +17921,7 @@
       </c>
       <c r="B192" s="88"/>
       <c r="C192" s="88"/>
-      <c r="D192" s="318"/>
+      <c r="D192" s="251"/>
       <c r="E192" s="154">
         <f t="array" ref="E192">MIN(IF(($B$8:$B$180=B192)*($D$8:$D$180=D192), $E$8:$E$180))</f>
         <v>0</v>
@@ -17889,9 +17942,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J192" s="270"/>
-      <c r="K192" s="271"/>
-      <c r="L192" s="271"/>
+      <c r="J192" s="278"/>
+      <c r="K192" s="279"/>
+      <c r="L192" s="279"/>
     </row>
     <row r="193" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A193" s="226">
@@ -17899,7 +17952,7 @@
       </c>
       <c r="B193" s="88"/>
       <c r="C193" s="88"/>
-      <c r="D193" s="318"/>
+      <c r="D193" s="251"/>
       <c r="E193" s="154">
         <f t="array" ref="E193">MIN(IF(($B$8:$B$180=B193)*($D$8:$D$180=D193), $E$8:$E$180))</f>
         <v>0</v>
@@ -17920,9 +17973,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J193" s="270"/>
-      <c r="K193" s="271"/>
-      <c r="L193" s="271"/>
+      <c r="J193" s="278"/>
+      <c r="K193" s="279"/>
+      <c r="L193" s="279"/>
     </row>
     <row r="194" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A194" s="226">
@@ -17930,7 +17983,7 @@
       </c>
       <c r="B194" s="88"/>
       <c r="C194" s="88"/>
-      <c r="D194" s="318"/>
+      <c r="D194" s="251"/>
       <c r="E194" s="154">
         <f t="array" ref="E194">MIN(IF(($B$8:$B$180=B194)*($D$8:$D$180=D194), $E$8:$E$180))</f>
         <v>0</v>
@@ -17951,9 +18004,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J194" s="270"/>
-      <c r="K194" s="271"/>
-      <c r="L194" s="271"/>
+      <c r="J194" s="278"/>
+      <c r="K194" s="279"/>
+      <c r="L194" s="279"/>
     </row>
     <row r="195" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A195" s="226">
@@ -17961,7 +18014,7 @@
       </c>
       <c r="B195" s="88"/>
       <c r="C195" s="88"/>
-      <c r="D195" s="318"/>
+      <c r="D195" s="251"/>
       <c r="E195" s="154">
         <f t="array" ref="E195">MIN(IF(($B$8:$B$180=B195)*($D$8:$D$180=D195), $E$8:$E$180))</f>
         <v>0</v>
@@ -17982,9 +18035,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J195" s="270"/>
-      <c r="K195" s="271"/>
-      <c r="L195" s="271"/>
+      <c r="J195" s="278"/>
+      <c r="K195" s="279"/>
+      <c r="L195" s="279"/>
     </row>
     <row r="196" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A196" s="226">
@@ -17992,7 +18045,7 @@
       </c>
       <c r="B196" s="88"/>
       <c r="C196" s="88"/>
-      <c r="D196" s="318"/>
+      <c r="D196" s="251"/>
       <c r="E196" s="154">
         <f t="array" ref="E196">MIN(IF(($B$8:$B$180=B196)*($D$8:$D$180=D196), $E$8:$E$180))</f>
         <v>0</v>
@@ -18013,9 +18066,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J196" s="270"/>
-      <c r="K196" s="271"/>
-      <c r="L196" s="271"/>
+      <c r="J196" s="278"/>
+      <c r="K196" s="279"/>
+      <c r="L196" s="279"/>
     </row>
     <row r="197" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A197" s="226">
@@ -18023,7 +18076,7 @@
       </c>
       <c r="B197" s="88"/>
       <c r="C197" s="88"/>
-      <c r="D197" s="318"/>
+      <c r="D197" s="251"/>
       <c r="E197" s="154">
         <f t="array" ref="E197">MIN(IF(($B$8:$B$180=B197)*($D$8:$D$180=D197), $E$8:$E$180))</f>
         <v>0</v>
@@ -18044,9 +18097,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J197" s="270"/>
-      <c r="K197" s="271"/>
-      <c r="L197" s="271"/>
+      <c r="J197" s="278"/>
+      <c r="K197" s="279"/>
+      <c r="L197" s="279"/>
     </row>
     <row r="198" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A198" s="226">
@@ -18054,7 +18107,7 @@
       </c>
       <c r="B198" s="88"/>
       <c r="C198" s="88"/>
-      <c r="D198" s="318"/>
+      <c r="D198" s="251"/>
       <c r="E198" s="154">
         <f t="array" ref="E198">MIN(IF(($B$8:$B$180=B198)*($D$8:$D$180=D198), $E$8:$E$180))</f>
         <v>0</v>
@@ -18075,9 +18128,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J198" s="270"/>
-      <c r="K198" s="271"/>
-      <c r="L198" s="271"/>
+      <c r="J198" s="278"/>
+      <c r="K198" s="279"/>
+      <c r="L198" s="279"/>
     </row>
     <row r="199" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A199" s="226">
@@ -18085,7 +18138,7 @@
       </c>
       <c r="B199" s="88"/>
       <c r="C199" s="88"/>
-      <c r="D199" s="318"/>
+      <c r="D199" s="251"/>
       <c r="E199" s="154">
         <f t="array" ref="E199">MIN(IF(($B$8:$B$180=B199)*($D$8:$D$180=D199), $E$8:$E$180))</f>
         <v>0</v>
@@ -18106,9 +18159,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J199" s="270"/>
-      <c r="K199" s="271"/>
-      <c r="L199" s="271"/>
+      <c r="J199" s="278"/>
+      <c r="K199" s="279"/>
+      <c r="L199" s="279"/>
     </row>
     <row r="200" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A200" s="226">
@@ -18116,7 +18169,7 @@
       </c>
       <c r="B200" s="88"/>
       <c r="C200" s="88"/>
-      <c r="D200" s="318"/>
+      <c r="D200" s="251"/>
       <c r="E200" s="154">
         <f t="array" ref="E200">MIN(IF(($B$8:$B$180=B200)*($D$8:$D$180=D200), $E$8:$E$180))</f>
         <v>0</v>
@@ -18137,9 +18190,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J200" s="270"/>
-      <c r="K200" s="271"/>
-      <c r="L200" s="271"/>
+      <c r="J200" s="278"/>
+      <c r="K200" s="279"/>
+      <c r="L200" s="279"/>
     </row>
     <row r="201" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A201" s="226">
@@ -18147,7 +18200,7 @@
       </c>
       <c r="B201" s="88"/>
       <c r="C201" s="88"/>
-      <c r="D201" s="318"/>
+      <c r="D201" s="251"/>
       <c r="E201" s="154">
         <f t="array" ref="E201">MIN(IF(($B$8:$B$180=B201)*($D$8:$D$180=D201), $E$8:$E$180))</f>
         <v>0</v>
@@ -18168,9 +18221,9 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J201" s="270"/>
-      <c r="K201" s="271"/>
-      <c r="L201" s="271"/>
+      <c r="J201" s="278"/>
+      <c r="K201" s="279"/>
+      <c r="L201" s="279"/>
     </row>
     <row r="202" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A202" s="227">
@@ -18178,7 +18231,7 @@
       </c>
       <c r="B202" s="147"/>
       <c r="C202" s="147"/>
-      <c r="D202" s="319"/>
+      <c r="D202" s="252"/>
       <c r="E202" s="222">
         <f t="array" ref="E202">MIN(IF(($B$8:$B$180=B202)*($D$8:$D$180=D202), $E$8:$E$180))</f>
         <v>0</v>
@@ -18199,17 +18252,17 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J202" s="278"/>
-      <c r="K202" s="279"/>
-      <c r="L202" s="279"/>
+      <c r="J202" s="276"/>
+      <c r="K202" s="277"/>
+      <c r="L202" s="277"/>
     </row>
     <row r="203" spans="1:14" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A203" s="288" t="s">
+      <c r="A203" s="290" t="s">
         <v>397</v>
       </c>
-      <c r="B203" s="273"/>
-      <c r="C203" s="273"/>
-      <c r="D203" s="274"/>
+      <c r="B203" s="288"/>
+      <c r="C203" s="288"/>
+      <c r="D203" s="289"/>
       <c r="E203" s="172"/>
       <c r="F203" s="159">
         <f>SUM(F185:F202)</f>
@@ -18228,8 +18281,8 @@
         <v>0</v>
       </c>
       <c r="J203" s="287"/>
-      <c r="K203" s="273"/>
-      <c r="L203" s="274"/>
+      <c r="K203" s="288"/>
+      <c r="L203" s="289"/>
     </row>
     <row r="204" spans="1:14" s="20" customFormat="1" ht="12.95" customHeight="1">
       <c r="A204" s="232"/>
@@ -18299,12 +18352,23 @@
     <row r="211" spans="4:12" ht="15" customHeight="1">
       <c r="D211" s="27"/>
       <c r="E211" s="81"/>
-      <c r="J211" s="277"/>
-      <c r="K211" s="276"/>
-      <c r="L211" s="276"/>
+      <c r="J211" s="274"/>
+      <c r="K211" s="275"/>
+      <c r="L211" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="J201:L201"/>
+    <mergeCell ref="J192:L192"/>
+    <mergeCell ref="J198:L198"/>
+    <mergeCell ref="J189:L189"/>
+    <mergeCell ref="J185:L185"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J191:L191"/>
+    <mergeCell ref="J187:L187"/>
+    <mergeCell ref="J196:L196"/>
+    <mergeCell ref="J193:L193"/>
     <mergeCell ref="J211:L211"/>
     <mergeCell ref="J202:L202"/>
     <mergeCell ref="J195:L195"/>
@@ -18321,17 +18385,6 @@
     <mergeCell ref="J200:L200"/>
     <mergeCell ref="A203:D203"/>
     <mergeCell ref="J197:L197"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J191:L191"/>
-    <mergeCell ref="J187:L187"/>
-    <mergeCell ref="J196:L196"/>
-    <mergeCell ref="J193:L193"/>
-    <mergeCell ref="J201:L201"/>
-    <mergeCell ref="J192:L192"/>
-    <mergeCell ref="J198:L198"/>
-    <mergeCell ref="J189:L189"/>
-    <mergeCell ref="J185:L185"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -18353,8 +18406,8 @@
   </sheetPr>
   <dimension ref="A1:M244"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A168" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185:D198"/>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="A139" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="L180" sqref="L180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -18381,14 +18434,14 @@
       <c r="D1" s="280" t="s">
         <v>364</v>
       </c>
-      <c r="E1" s="276"/>
-      <c r="F1" s="276"/>
-      <c r="G1" s="276"/>
-      <c r="H1" s="276"/>
-      <c r="I1" s="276"/>
-      <c r="J1" s="276"/>
-      <c r="K1" s="276"/>
-      <c r="L1" s="276"/>
+      <c r="E1" s="275"/>
+      <c r="F1" s="275"/>
+      <c r="G1" s="275"/>
+      <c r="H1" s="275"/>
+      <c r="I1" s="275"/>
+      <c r="J1" s="275"/>
+      <c r="K1" s="275"/>
+      <c r="L1" s="275"/>
     </row>
     <row r="2" spans="1:12">
       <c r="B2" s="11"/>
@@ -18423,9 +18476,9 @@
         <v>369</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="275"/>
-      <c r="K4" s="276"/>
-      <c r="L4" s="276"/>
+      <c r="J4" s="292"/>
+      <c r="K4" s="275"/>
+      <c r="L4" s="275"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="B5" s="10" t="s">
@@ -21940,12 +21993,12 @@
       </c>
     </row>
     <row r="180" spans="1:12" ht="21.75" customHeight="1">
-      <c r="A180" s="300" t="s">
+      <c r="A180" s="309" t="s">
         <v>386</v>
       </c>
-      <c r="B180" s="273"/>
-      <c r="C180" s="273"/>
-      <c r="D180" s="274"/>
+      <c r="B180" s="288"/>
+      <c r="C180" s="288"/>
+      <c r="D180" s="289"/>
       <c r="E180" s="149"/>
       <c r="F180" s="164">
         <f>SUM(F8:F179)</f>
@@ -21988,17 +22041,17 @@
       <c r="A182" s="281" t="s">
         <v>405</v>
       </c>
-      <c r="B182" s="276"/>
-      <c r="C182" s="276"/>
-      <c r="D182" s="276"/>
-      <c r="E182" s="276"/>
-      <c r="F182" s="276"/>
-      <c r="G182" s="276"/>
-      <c r="H182" s="276"/>
-      <c r="I182" s="276"/>
-      <c r="J182" s="276"/>
-      <c r="K182" s="276"/>
-      <c r="L182" s="276"/>
+      <c r="B182" s="275"/>
+      <c r="C182" s="275"/>
+      <c r="D182" s="275"/>
+      <c r="E182" s="275"/>
+      <c r="F182" s="275"/>
+      <c r="G182" s="275"/>
+      <c r="H182" s="275"/>
+      <c r="I182" s="275"/>
+      <c r="J182" s="275"/>
+      <c r="K182" s="275"/>
+      <c r="L182" s="275"/>
     </row>
     <row r="183" spans="1:12" s="20" customFormat="1" ht="12.95" customHeight="1">
       <c r="A183" s="232"/>
@@ -22042,11 +22095,11 @@
       <c r="I184" s="177" t="s">
         <v>395</v>
       </c>
-      <c r="J184" s="313" t="s">
+      <c r="J184" s="300" t="s">
         <v>396</v>
       </c>
-      <c r="K184" s="273"/>
-      <c r="L184" s="274"/>
+      <c r="K184" s="288"/>
+      <c r="L184" s="289"/>
     </row>
     <row r="185" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A185" s="225">
@@ -22054,7 +22107,7 @@
       </c>
       <c r="B185" s="174"/>
       <c r="C185" s="174"/>
-      <c r="D185" s="317"/>
+      <c r="D185" s="250"/>
       <c r="E185" s="175">
         <f t="array" ref="E185">MIN(IF(($B$8:$B$180=B185)*($D$8:$D$180=D185), $E$8:$E$180))</f>
         <v>0</v>
@@ -22071,10 +22124,13 @@
         <f t="shared" ref="H185:H198" si="8">SUMIFS($H$8:$H$180, $B$8:$B$180,B185,$D$8:$D$180,D185)</f>
         <v>0</v>
       </c>
-      <c r="I185" s="176"/>
-      <c r="J185" s="309"/>
-      <c r="K185" s="310"/>
-      <c r="L185" s="311"/>
+      <c r="I185" s="155">
+        <f t="shared" ref="I185:I198" si="9">SUMIFS($L$8:$L$180, $B$8:$B$180,B185,$D$8:$D$180,D185)</f>
+        <v>0</v>
+      </c>
+      <c r="J185" s="315"/>
+      <c r="K185" s="316"/>
+      <c r="L185" s="317"/>
     </row>
     <row r="186" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A186" s="226">
@@ -22082,7 +22138,7 @@
       </c>
       <c r="B186" s="88"/>
       <c r="C186" s="88"/>
-      <c r="D186" s="318"/>
+      <c r="D186" s="251"/>
       <c r="E186" s="154">
         <f t="array" ref="E186">MIN(IF(($B$8:$B$180=B186)*($D$8:$D$180=D186), $E$8:$E$180))</f>
         <v>0</v>
@@ -22100,12 +22156,12 @@
         <v>0</v>
       </c>
       <c r="I186" s="155">
-        <f t="shared" ref="I186:I198" si="9">SUMIFS($L$8:$L$180, $B$8:$B$180,B186,$D$8:$D$180,D186)</f>
-        <v>0</v>
-      </c>
-      <c r="J186" s="270"/>
-      <c r="K186" s="301"/>
-      <c r="L186" s="302"/>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J186" s="278"/>
+      <c r="K186" s="293"/>
+      <c r="L186" s="294"/>
     </row>
     <row r="187" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A187" s="226">
@@ -22113,7 +22169,7 @@
       </c>
       <c r="B187" s="88"/>
       <c r="C187" s="88"/>
-      <c r="D187" s="318"/>
+      <c r="D187" s="251"/>
       <c r="E187" s="154">
         <f t="array" ref="E187">MIN(IF(($B$8:$B$180=B187)*($D$8:$D$180=D187), $E$8:$E$180))</f>
         <v>0</v>
@@ -22134,9 +22190,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J187" s="270"/>
-      <c r="K187" s="301"/>
-      <c r="L187" s="302"/>
+      <c r="J187" s="278"/>
+      <c r="K187" s="293"/>
+      <c r="L187" s="294"/>
     </row>
     <row r="188" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A188" s="226">
@@ -22144,7 +22200,7 @@
       </c>
       <c r="B188" s="88"/>
       <c r="C188" s="88"/>
-      <c r="D188" s="318"/>
+      <c r="D188" s="251"/>
       <c r="E188" s="154">
         <f t="array" ref="E188">MIN(IF(($B$8:$B$180=B188)*($D$8:$D$180=D188), $E$8:$E$180))</f>
         <v>0</v>
@@ -22165,9 +22221,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J188" s="270"/>
-      <c r="K188" s="301"/>
-      <c r="L188" s="302"/>
+      <c r="J188" s="278"/>
+      <c r="K188" s="293"/>
+      <c r="L188" s="294"/>
     </row>
     <row r="189" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A189" s="226">
@@ -22175,7 +22231,7 @@
       </c>
       <c r="B189" s="88"/>
       <c r="C189" s="88"/>
-      <c r="D189" s="318"/>
+      <c r="D189" s="251"/>
       <c r="E189" s="154">
         <f t="array" ref="E189">MIN(IF(($B$8:$B$180=B189)*($D$8:$D$180=D189), $E$8:$E$180))</f>
         <v>0</v>
@@ -22196,9 +22252,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J189" s="270"/>
-      <c r="K189" s="301"/>
-      <c r="L189" s="302"/>
+      <c r="J189" s="278"/>
+      <c r="K189" s="293"/>
+      <c r="L189" s="294"/>
     </row>
     <row r="190" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A190" s="226">
@@ -22206,7 +22262,7 @@
       </c>
       <c r="B190" s="88"/>
       <c r="C190" s="88"/>
-      <c r="D190" s="318"/>
+      <c r="D190" s="251"/>
       <c r="E190" s="154">
         <f t="array" ref="E190">MIN(IF(($B$8:$B$180=B190)*($D$8:$D$180=D190), $E$8:$E$180))</f>
         <v>0</v>
@@ -22227,9 +22283,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J190" s="270"/>
-      <c r="K190" s="301"/>
-      <c r="L190" s="302"/>
+      <c r="J190" s="278"/>
+      <c r="K190" s="293"/>
+      <c r="L190" s="294"/>
     </row>
     <row r="191" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A191" s="226">
@@ -22237,7 +22293,7 @@
       </c>
       <c r="B191" s="88"/>
       <c r="C191" s="88"/>
-      <c r="D191" s="318"/>
+      <c r="D191" s="251"/>
       <c r="E191" s="154">
         <f t="array" ref="E191">MIN(IF(($B$8:$B$180=B191)*($D$8:$D$180=D191), $E$8:$E$180))</f>
         <v>0</v>
@@ -22258,9 +22314,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J191" s="270"/>
-      <c r="K191" s="301"/>
-      <c r="L191" s="302"/>
+      <c r="J191" s="278"/>
+      <c r="K191" s="293"/>
+      <c r="L191" s="294"/>
     </row>
     <row r="192" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A192" s="226">
@@ -22268,7 +22324,7 @@
       </c>
       <c r="B192" s="88"/>
       <c r="C192" s="88"/>
-      <c r="D192" s="318"/>
+      <c r="D192" s="251"/>
       <c r="E192" s="154">
         <f t="array" ref="E192">MIN(IF(($B$8:$B$180=B192)*($D$8:$D$180=D192), $E$8:$E$180))</f>
         <v>0</v>
@@ -22289,9 +22345,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J192" s="270"/>
-      <c r="K192" s="301"/>
-      <c r="L192" s="302"/>
+      <c r="J192" s="278"/>
+      <c r="K192" s="293"/>
+      <c r="L192" s="294"/>
     </row>
     <row r="193" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A193" s="226">
@@ -22299,7 +22355,7 @@
       </c>
       <c r="B193" s="88"/>
       <c r="C193" s="88"/>
-      <c r="D193" s="318"/>
+      <c r="D193" s="251"/>
       <c r="E193" s="154">
         <f t="array" ref="E193">MIN(IF(($B$8:$B$180=B193)*($D$8:$D$180=D193), $E$8:$E$180))</f>
         <v>0</v>
@@ -22320,9 +22376,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J193" s="270"/>
-      <c r="K193" s="301"/>
-      <c r="L193" s="302"/>
+      <c r="J193" s="278"/>
+      <c r="K193" s="293"/>
+      <c r="L193" s="294"/>
     </row>
     <row r="194" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A194" s="226">
@@ -22330,7 +22386,7 @@
       </c>
       <c r="B194" s="88"/>
       <c r="C194" s="88"/>
-      <c r="D194" s="318"/>
+      <c r="D194" s="251"/>
       <c r="E194" s="154">
         <f t="array" ref="E194">MIN(IF(($B$8:$B$180=B194)*($D$8:$D$180=D194), $E$8:$E$180))</f>
         <v>0</v>
@@ -22351,9 +22407,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J194" s="270"/>
-      <c r="K194" s="301"/>
-      <c r="L194" s="302"/>
+      <c r="J194" s="278"/>
+      <c r="K194" s="293"/>
+      <c r="L194" s="294"/>
     </row>
     <row r="195" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A195" s="226">
@@ -22361,7 +22417,7 @@
       </c>
       <c r="B195" s="88"/>
       <c r="C195" s="88"/>
-      <c r="D195" s="318"/>
+      <c r="D195" s="251"/>
       <c r="E195" s="154">
         <f t="array" ref="E195">MIN(IF(($B$8:$B$180=B195)*($D$8:$D$180=D195), $E$8:$E$180))</f>
         <v>0</v>
@@ -22382,9 +22438,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J195" s="270"/>
-      <c r="K195" s="301"/>
-      <c r="L195" s="302"/>
+      <c r="J195" s="278"/>
+      <c r="K195" s="293"/>
+      <c r="L195" s="294"/>
     </row>
     <row r="196" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A196" s="226">
@@ -22392,7 +22448,7 @@
       </c>
       <c r="B196" s="88"/>
       <c r="C196" s="88"/>
-      <c r="D196" s="318"/>
+      <c r="D196" s="251"/>
       <c r="E196" s="154">
         <f t="array" ref="E196">MIN(IF(($B$8:$B$180=B196)*($D$8:$D$180=D196), $E$8:$E$180))</f>
         <v>0</v>
@@ -22413,9 +22469,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J196" s="270"/>
-      <c r="K196" s="301"/>
-      <c r="L196" s="302"/>
+      <c r="J196" s="278"/>
+      <c r="K196" s="293"/>
+      <c r="L196" s="294"/>
     </row>
     <row r="197" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A197" s="226">
@@ -22423,7 +22479,7 @@
       </c>
       <c r="B197" s="88"/>
       <c r="C197" s="88"/>
-      <c r="D197" s="318"/>
+      <c r="D197" s="251"/>
       <c r="E197" s="154">
         <f t="array" ref="E197">MIN(IF(($B$8:$B$180=B197)*($D$8:$D$180=D197), $E$8:$E$180))</f>
         <v>0</v>
@@ -22444,9 +22500,9 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J197" s="270"/>
-      <c r="K197" s="301"/>
-      <c r="L197" s="302"/>
+      <c r="J197" s="278"/>
+      <c r="K197" s="293"/>
+      <c r="L197" s="294"/>
     </row>
     <row r="198" spans="1:12" s="20" customFormat="1" ht="15" customHeight="1">
       <c r="A198" s="227">
@@ -22454,7 +22510,7 @@
       </c>
       <c r="B198" s="147"/>
       <c r="C198" s="147"/>
-      <c r="D198" s="319"/>
+      <c r="D198" s="252"/>
       <c r="E198" s="154">
         <f t="array" ref="E198">MIN(IF(($B$8:$B$180=B198)*($D$8:$D$180=D198), $E$8:$E$180))</f>
         <v>0</v>
@@ -22475,17 +22531,17 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J198" s="278"/>
-      <c r="K198" s="305"/>
-      <c r="L198" s="306"/>
+      <c r="J198" s="276"/>
+      <c r="K198" s="313"/>
+      <c r="L198" s="314"/>
     </row>
     <row r="199" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
-      <c r="A199" s="288" t="s">
+      <c r="A199" s="290" t="s">
         <v>397</v>
       </c>
-      <c r="B199" s="273"/>
-      <c r="C199" s="273"/>
-      <c r="D199" s="274"/>
+      <c r="B199" s="288"/>
+      <c r="C199" s="288"/>
+      <c r="D199" s="289"/>
       <c r="E199" s="168"/>
       <c r="F199" s="159">
         <f>SUM(F185:F198)</f>
@@ -22503,9 +22559,9 @@
         <f>SUM(I185:I198)</f>
         <v>0</v>
       </c>
-      <c r="J199" s="314"/>
-      <c r="K199" s="273"/>
-      <c r="L199" s="274"/>
+      <c r="J199" s="295"/>
+      <c r="K199" s="288"/>
+      <c r="L199" s="289"/>
     </row>
     <row r="200" spans="1:12" s="20" customFormat="1" ht="12.95" customHeight="1">
       <c r="A200" s="232"/>
@@ -22522,20 +22578,20 @@
       <c r="L200" s="83"/>
     </row>
     <row r="201" spans="1:12" ht="15.95" customHeight="1">
-      <c r="A201" s="312" t="s">
+      <c r="A201" s="305" t="s">
         <v>406</v>
       </c>
-      <c r="B201" s="276"/>
-      <c r="C201" s="276"/>
-      <c r="D201" s="276"/>
-      <c r="E201" s="276"/>
-      <c r="F201" s="276"/>
-      <c r="G201" s="276"/>
-      <c r="H201" s="276"/>
-      <c r="I201" s="276"/>
-      <c r="J201" s="276"/>
-      <c r="K201" s="276"/>
-      <c r="L201" s="276"/>
+      <c r="B201" s="275"/>
+      <c r="C201" s="275"/>
+      <c r="D201" s="275"/>
+      <c r="E201" s="275"/>
+      <c r="F201" s="275"/>
+      <c r="G201" s="275"/>
+      <c r="H201" s="275"/>
+      <c r="I201" s="275"/>
+      <c r="J201" s="275"/>
+      <c r="K201" s="275"/>
+      <c r="L201" s="275"/>
     </row>
     <row r="202" spans="1:12" ht="12.95" customHeight="1">
       <c r="B202" s="30"/>
@@ -22554,20 +22610,20 @@
       <c r="A203" s="233" t="s">
         <v>388</v>
       </c>
-      <c r="B203" s="313" t="s">
+      <c r="B203" s="300" t="s">
         <v>407</v>
       </c>
-      <c r="C203" s="274"/>
-      <c r="D203" s="293" t="s">
+      <c r="C203" s="289"/>
+      <c r="D203" s="310" t="s">
         <v>408</v>
       </c>
-      <c r="E203" s="273"/>
-      <c r="F203" s="273"/>
-      <c r="G203" s="273"/>
-      <c r="H203" s="273"/>
-      <c r="I203" s="273"/>
-      <c r="J203" s="273"/>
-      <c r="K203" s="274"/>
+      <c r="E203" s="288"/>
+      <c r="F203" s="288"/>
+      <c r="G203" s="288"/>
+      <c r="H203" s="288"/>
+      <c r="I203" s="288"/>
+      <c r="J203" s="288"/>
+      <c r="K203" s="289"/>
       <c r="L203" s="18" t="s">
         <v>409</v>
       </c>
@@ -22576,196 +22632,196 @@
       <c r="A204" s="242">
         <v>1</v>
       </c>
-      <c r="B204" s="307"/>
-      <c r="C204" s="308"/>
-      <c r="D204" s="303"/>
-      <c r="E204" s="292"/>
-      <c r="F204" s="292"/>
-      <c r="G204" s="292"/>
-      <c r="H204" s="292"/>
-      <c r="I204" s="292"/>
-      <c r="J204" s="292"/>
-      <c r="K204" s="290"/>
+      <c r="B204" s="298"/>
+      <c r="C204" s="299"/>
+      <c r="D204" s="311"/>
+      <c r="E204" s="312"/>
+      <c r="F204" s="312"/>
+      <c r="G204" s="312"/>
+      <c r="H204" s="312"/>
+      <c r="I204" s="312"/>
+      <c r="J204" s="312"/>
+      <c r="K204" s="297"/>
       <c r="L204" s="119"/>
     </row>
     <row r="205" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A205" s="226">
         <v>2</v>
       </c>
-      <c r="B205" s="307"/>
-      <c r="C205" s="308"/>
-      <c r="D205" s="297"/>
-      <c r="E205" s="298"/>
-      <c r="F205" s="298"/>
-      <c r="G205" s="298"/>
-      <c r="H205" s="298"/>
-      <c r="I205" s="298"/>
-      <c r="J205" s="298"/>
-      <c r="K205" s="299"/>
+      <c r="B205" s="321"/>
+      <c r="C205" s="322"/>
+      <c r="D205" s="301"/>
+      <c r="E205" s="302"/>
+      <c r="F205" s="302"/>
+      <c r="G205" s="302"/>
+      <c r="H205" s="302"/>
+      <c r="I205" s="302"/>
+      <c r="J205" s="302"/>
+      <c r="K205" s="303"/>
       <c r="L205" s="120"/>
     </row>
     <row r="206" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A206" s="226">
         <v>3</v>
       </c>
-      <c r="B206" s="307"/>
-      <c r="C206" s="308"/>
+      <c r="B206" s="321"/>
+      <c r="C206" s="322"/>
       <c r="D206" s="304"/>
-      <c r="E206" s="298"/>
-      <c r="F206" s="298"/>
-      <c r="G206" s="298"/>
-      <c r="H206" s="298"/>
-      <c r="I206" s="298"/>
-      <c r="J206" s="298"/>
-      <c r="K206" s="299"/>
+      <c r="E206" s="302"/>
+      <c r="F206" s="302"/>
+      <c r="G206" s="302"/>
+      <c r="H206" s="302"/>
+      <c r="I206" s="302"/>
+      <c r="J206" s="302"/>
+      <c r="K206" s="303"/>
       <c r="L206" s="121"/>
     </row>
     <row r="207" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A207" s="226">
         <v>4</v>
       </c>
-      <c r="B207" s="307"/>
-      <c r="C207" s="308"/>
-      <c r="D207" s="297"/>
-      <c r="E207" s="298"/>
-      <c r="F207" s="298"/>
-      <c r="G207" s="298"/>
-      <c r="H207" s="298"/>
-      <c r="I207" s="298"/>
-      <c r="J207" s="298"/>
-      <c r="K207" s="299"/>
+      <c r="B207" s="321"/>
+      <c r="C207" s="322"/>
+      <c r="D207" s="301"/>
+      <c r="E207" s="302"/>
+      <c r="F207" s="302"/>
+      <c r="G207" s="302"/>
+      <c r="H207" s="302"/>
+      <c r="I207" s="302"/>
+      <c r="J207" s="302"/>
+      <c r="K207" s="303"/>
       <c r="L207" s="120"/>
     </row>
     <row r="208" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A208" s="226">
         <v>5</v>
       </c>
-      <c r="B208" s="307"/>
-      <c r="C208" s="308"/>
-      <c r="D208" s="297"/>
-      <c r="E208" s="298"/>
-      <c r="F208" s="298"/>
-      <c r="G208" s="298"/>
-      <c r="H208" s="298"/>
-      <c r="I208" s="298"/>
-      <c r="J208" s="298"/>
-      <c r="K208" s="299"/>
+      <c r="B208" s="321"/>
+      <c r="C208" s="322"/>
+      <c r="D208" s="301"/>
+      <c r="E208" s="302"/>
+      <c r="F208" s="302"/>
+      <c r="G208" s="302"/>
+      <c r="H208" s="302"/>
+      <c r="I208" s="302"/>
+      <c r="J208" s="302"/>
+      <c r="K208" s="303"/>
       <c r="L208" s="120"/>
     </row>
     <row r="209" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A209" s="226">
         <v>6</v>
       </c>
-      <c r="B209" s="307"/>
-      <c r="C209" s="308"/>
-      <c r="D209" s="297"/>
-      <c r="E209" s="298"/>
-      <c r="F209" s="298"/>
-      <c r="G209" s="298"/>
-      <c r="H209" s="298"/>
-      <c r="I209" s="298"/>
-      <c r="J209" s="298"/>
-      <c r="K209" s="299"/>
+      <c r="B209" s="321"/>
+      <c r="C209" s="322"/>
+      <c r="D209" s="301"/>
+      <c r="E209" s="302"/>
+      <c r="F209" s="302"/>
+      <c r="G209" s="302"/>
+      <c r="H209" s="302"/>
+      <c r="I209" s="302"/>
+      <c r="J209" s="302"/>
+      <c r="K209" s="303"/>
       <c r="L209" s="120"/>
     </row>
     <row r="210" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A210" s="226">
         <v>7</v>
       </c>
-      <c r="B210" s="307"/>
-      <c r="C210" s="308"/>
-      <c r="D210" s="297"/>
-      <c r="E210" s="298"/>
-      <c r="F210" s="298"/>
-      <c r="G210" s="298"/>
-      <c r="H210" s="298"/>
-      <c r="I210" s="298"/>
-      <c r="J210" s="298"/>
-      <c r="K210" s="299"/>
+      <c r="B210" s="321"/>
+      <c r="C210" s="322"/>
+      <c r="D210" s="301"/>
+      <c r="E210" s="302"/>
+      <c r="F210" s="302"/>
+      <c r="G210" s="302"/>
+      <c r="H210" s="302"/>
+      <c r="I210" s="302"/>
+      <c r="J210" s="302"/>
+      <c r="K210" s="303"/>
       <c r="L210" s="120"/>
     </row>
     <row r="211" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A211" s="226">
         <v>8</v>
       </c>
-      <c r="B211" s="307"/>
-      <c r="C211" s="308"/>
-      <c r="D211" s="297"/>
-      <c r="E211" s="298"/>
-      <c r="F211" s="298"/>
-      <c r="G211" s="298"/>
-      <c r="H211" s="298"/>
-      <c r="I211" s="298"/>
-      <c r="J211" s="298"/>
-      <c r="K211" s="299"/>
+      <c r="B211" s="321"/>
+      <c r="C211" s="322"/>
+      <c r="D211" s="301"/>
+      <c r="E211" s="302"/>
+      <c r="F211" s="302"/>
+      <c r="G211" s="302"/>
+      <c r="H211" s="302"/>
+      <c r="I211" s="302"/>
+      <c r="J211" s="302"/>
+      <c r="K211" s="303"/>
       <c r="L211" s="120"/>
     </row>
     <row r="212" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A212" s="226">
         <v>9</v>
       </c>
-      <c r="B212" s="307"/>
-      <c r="C212" s="308"/>
-      <c r="D212" s="297"/>
-      <c r="E212" s="298"/>
-      <c r="F212" s="298"/>
-      <c r="G212" s="298"/>
-      <c r="H212" s="298"/>
-      <c r="I212" s="298"/>
-      <c r="J212" s="298"/>
-      <c r="K212" s="299"/>
+      <c r="B212" s="321"/>
+      <c r="C212" s="322"/>
+      <c r="D212" s="301"/>
+      <c r="E212" s="302"/>
+      <c r="F212" s="302"/>
+      <c r="G212" s="302"/>
+      <c r="H212" s="302"/>
+      <c r="I212" s="302"/>
+      <c r="J212" s="302"/>
+      <c r="K212" s="303"/>
       <c r="L212" s="120"/>
     </row>
     <row r="213" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A213" s="227">
         <v>10</v>
       </c>
-      <c r="B213" s="307"/>
-      <c r="C213" s="308"/>
-      <c r="D213" s="294"/>
-      <c r="E213" s="295"/>
-      <c r="F213" s="295"/>
-      <c r="G213" s="295"/>
-      <c r="H213" s="295"/>
-      <c r="I213" s="295"/>
-      <c r="J213" s="295"/>
-      <c r="K213" s="296"/>
+      <c r="B213" s="323"/>
+      <c r="C213" s="324"/>
+      <c r="D213" s="306"/>
+      <c r="E213" s="307"/>
+      <c r="F213" s="307"/>
+      <c r="G213" s="307"/>
+      <c r="H213" s="307"/>
+      <c r="I213" s="307"/>
+      <c r="J213" s="307"/>
+      <c r="K213" s="308"/>
       <c r="L213" s="122"/>
     </row>
     <row r="214" spans="1:12" ht="15" customHeight="1">
-      <c r="A214" s="272" t="s">
+      <c r="A214" s="291" t="s">
         <v>386</v>
       </c>
-      <c r="B214" s="273"/>
-      <c r="C214" s="273"/>
-      <c r="D214" s="273"/>
-      <c r="E214" s="273"/>
-      <c r="F214" s="273"/>
-      <c r="G214" s="273"/>
-      <c r="H214" s="273"/>
-      <c r="I214" s="273"/>
-      <c r="J214" s="273"/>
-      <c r="K214" s="274"/>
+      <c r="B214" s="288"/>
+      <c r="C214" s="288"/>
+      <c r="D214" s="288"/>
+      <c r="E214" s="288"/>
+      <c r="F214" s="288"/>
+      <c r="G214" s="288"/>
+      <c r="H214" s="288"/>
+      <c r="I214" s="288"/>
+      <c r="J214" s="288"/>
+      <c r="K214" s="289"/>
       <c r="L214" s="163">
         <f>SUM(L204:L213)</f>
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:12" ht="21.6" customHeight="1">
-      <c r="A215" s="312" t="s">
+      <c r="A215" s="305" t="s">
         <v>410</v>
       </c>
-      <c r="B215" s="276"/>
-      <c r="C215" s="276"/>
-      <c r="D215" s="276"/>
-      <c r="E215" s="276"/>
-      <c r="F215" s="276"/>
-      <c r="G215" s="276"/>
-      <c r="H215" s="276"/>
-      <c r="I215" s="276"/>
-      <c r="J215" s="276"/>
-      <c r="K215" s="276"/>
-      <c r="L215" s="276"/>
+      <c r="B215" s="275"/>
+      <c r="C215" s="275"/>
+      <c r="D215" s="275"/>
+      <c r="E215" s="275"/>
+      <c r="F215" s="275"/>
+      <c r="G215" s="275"/>
+      <c r="H215" s="275"/>
+      <c r="I215" s="275"/>
+      <c r="J215" s="275"/>
+      <c r="K215" s="275"/>
+      <c r="L215" s="275"/>
     </row>
     <row r="216" spans="1:12" ht="9" customHeight="1">
       <c r="B216" s="30"/>
@@ -22784,20 +22840,20 @@
       <c r="A217" s="233" t="s">
         <v>388</v>
       </c>
-      <c r="B217" s="313" t="s">
+      <c r="B217" s="300" t="s">
         <v>407</v>
       </c>
-      <c r="C217" s="274"/>
-      <c r="D217" s="293" t="s">
+      <c r="C217" s="289"/>
+      <c r="D217" s="310" t="s">
         <v>408</v>
       </c>
-      <c r="E217" s="273"/>
-      <c r="F217" s="273"/>
-      <c r="G217" s="273"/>
-      <c r="H217" s="273"/>
-      <c r="I217" s="273"/>
-      <c r="J217" s="273"/>
-      <c r="K217" s="274"/>
+      <c r="E217" s="288"/>
+      <c r="F217" s="288"/>
+      <c r="G217" s="288"/>
+      <c r="H217" s="288"/>
+      <c r="I217" s="288"/>
+      <c r="J217" s="288"/>
+      <c r="K217" s="289"/>
       <c r="L217" s="18" t="s">
         <v>409</v>
       </c>
@@ -22806,176 +22862,176 @@
       <c r="A218" s="242">
         <v>1</v>
       </c>
-      <c r="B218" s="289"/>
-      <c r="C218" s="290"/>
-      <c r="D218" s="291"/>
-      <c r="E218" s="292"/>
-      <c r="F218" s="292"/>
-      <c r="G218" s="292"/>
-      <c r="H218" s="292"/>
-      <c r="I218" s="292"/>
-      <c r="J218" s="292"/>
-      <c r="K218" s="290"/>
+      <c r="B218" s="296"/>
+      <c r="C218" s="297"/>
+      <c r="D218" s="318"/>
+      <c r="E218" s="312"/>
+      <c r="F218" s="312"/>
+      <c r="G218" s="312"/>
+      <c r="H218" s="312"/>
+      <c r="I218" s="312"/>
+      <c r="J218" s="312"/>
+      <c r="K218" s="297"/>
       <c r="L218" s="119"/>
     </row>
     <row r="219" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A219" s="226">
         <v>2</v>
       </c>
-      <c r="B219" s="289"/>
-      <c r="C219" s="290"/>
-      <c r="D219" s="297"/>
-      <c r="E219" s="298"/>
-      <c r="F219" s="298"/>
-      <c r="G219" s="298"/>
-      <c r="H219" s="298"/>
-      <c r="I219" s="298"/>
-      <c r="J219" s="298"/>
-      <c r="K219" s="299"/>
+      <c r="B219" s="325"/>
+      <c r="C219" s="303"/>
+      <c r="D219" s="301"/>
+      <c r="E219" s="302"/>
+      <c r="F219" s="302"/>
+      <c r="G219" s="302"/>
+      <c r="H219" s="302"/>
+      <c r="I219" s="302"/>
+      <c r="J219" s="302"/>
+      <c r="K219" s="303"/>
       <c r="L219" s="120"/>
     </row>
     <row r="220" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A220" s="226">
         <v>3</v>
       </c>
-      <c r="B220" s="289"/>
-      <c r="C220" s="290"/>
+      <c r="B220" s="325"/>
+      <c r="C220" s="303"/>
       <c r="D220" s="304"/>
-      <c r="E220" s="298"/>
-      <c r="F220" s="298"/>
-      <c r="G220" s="298"/>
-      <c r="H220" s="298"/>
-      <c r="I220" s="298"/>
-      <c r="J220" s="298"/>
-      <c r="K220" s="299"/>
+      <c r="E220" s="302"/>
+      <c r="F220" s="302"/>
+      <c r="G220" s="302"/>
+      <c r="H220" s="302"/>
+      <c r="I220" s="302"/>
+      <c r="J220" s="302"/>
+      <c r="K220" s="303"/>
       <c r="L220" s="121"/>
     </row>
     <row r="221" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A221" s="226">
         <v>4</v>
       </c>
-      <c r="B221" s="289"/>
-      <c r="C221" s="290"/>
-      <c r="D221" s="297"/>
-      <c r="E221" s="298"/>
-      <c r="F221" s="298"/>
-      <c r="G221" s="298"/>
-      <c r="H221" s="298"/>
-      <c r="I221" s="298"/>
-      <c r="J221" s="298"/>
-      <c r="K221" s="299"/>
+      <c r="B221" s="325"/>
+      <c r="C221" s="303"/>
+      <c r="D221" s="301"/>
+      <c r="E221" s="302"/>
+      <c r="F221" s="302"/>
+      <c r="G221" s="302"/>
+      <c r="H221" s="302"/>
+      <c r="I221" s="302"/>
+      <c r="J221" s="302"/>
+      <c r="K221" s="303"/>
       <c r="L221" s="120"/>
     </row>
     <row r="222" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A222" s="226">
         <v>5</v>
       </c>
-      <c r="B222" s="289"/>
-      <c r="C222" s="290"/>
-      <c r="D222" s="297"/>
-      <c r="E222" s="298"/>
-      <c r="F222" s="298"/>
-      <c r="G222" s="298"/>
-      <c r="H222" s="298"/>
-      <c r="I222" s="298"/>
-      <c r="J222" s="298"/>
-      <c r="K222" s="299"/>
+      <c r="B222" s="325"/>
+      <c r="C222" s="303"/>
+      <c r="D222" s="301"/>
+      <c r="E222" s="302"/>
+      <c r="F222" s="302"/>
+      <c r="G222" s="302"/>
+      <c r="H222" s="302"/>
+      <c r="I222" s="302"/>
+      <c r="J222" s="302"/>
+      <c r="K222" s="303"/>
       <c r="L222" s="120"/>
     </row>
     <row r="223" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A223" s="226">
         <v>6</v>
       </c>
-      <c r="B223" s="289"/>
-      <c r="C223" s="290"/>
-      <c r="D223" s="297"/>
-      <c r="E223" s="298"/>
-      <c r="F223" s="298"/>
-      <c r="G223" s="298"/>
-      <c r="H223" s="298"/>
-      <c r="I223" s="298"/>
-      <c r="J223" s="298"/>
-      <c r="K223" s="299"/>
+      <c r="B223" s="325"/>
+      <c r="C223" s="303"/>
+      <c r="D223" s="301"/>
+      <c r="E223" s="302"/>
+      <c r="F223" s="302"/>
+      <c r="G223" s="302"/>
+      <c r="H223" s="302"/>
+      <c r="I223" s="302"/>
+      <c r="J223" s="302"/>
+      <c r="K223" s="303"/>
       <c r="L223" s="120"/>
     </row>
     <row r="224" spans="1:12" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A224" s="226">
         <v>7</v>
       </c>
-      <c r="B224" s="289"/>
-      <c r="C224" s="290"/>
-      <c r="D224" s="297"/>
-      <c r="E224" s="298"/>
-      <c r="F224" s="298"/>
-      <c r="G224" s="298"/>
-      <c r="H224" s="298"/>
-      <c r="I224" s="298"/>
-      <c r="J224" s="298"/>
-      <c r="K224" s="299"/>
+      <c r="B224" s="325"/>
+      <c r="C224" s="303"/>
+      <c r="D224" s="301"/>
+      <c r="E224" s="302"/>
+      <c r="F224" s="302"/>
+      <c r="G224" s="302"/>
+      <c r="H224" s="302"/>
+      <c r="I224" s="302"/>
+      <c r="J224" s="302"/>
+      <c r="K224" s="303"/>
       <c r="L224" s="120"/>
     </row>
     <row r="225" spans="1:13" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A225" s="226">
         <v>8</v>
       </c>
-      <c r="B225" s="289"/>
-      <c r="C225" s="290"/>
-      <c r="D225" s="297"/>
-      <c r="E225" s="298"/>
-      <c r="F225" s="298"/>
-      <c r="G225" s="298"/>
-      <c r="H225" s="298"/>
-      <c r="I225" s="298"/>
-      <c r="J225" s="298"/>
-      <c r="K225" s="299"/>
+      <c r="B225" s="325"/>
+      <c r="C225" s="303"/>
+      <c r="D225" s="301"/>
+      <c r="E225" s="302"/>
+      <c r="F225" s="302"/>
+      <c r="G225" s="302"/>
+      <c r="H225" s="302"/>
+      <c r="I225" s="302"/>
+      <c r="J225" s="302"/>
+      <c r="K225" s="303"/>
       <c r="L225" s="120"/>
     </row>
     <row r="226" spans="1:13" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A226" s="226">
         <v>9</v>
       </c>
-      <c r="B226" s="289"/>
-      <c r="C226" s="290"/>
-      <c r="D226" s="297"/>
-      <c r="E226" s="298"/>
-      <c r="F226" s="298"/>
-      <c r="G226" s="298"/>
-      <c r="H226" s="298"/>
-      <c r="I226" s="298"/>
-      <c r="J226" s="298"/>
-      <c r="K226" s="299"/>
+      <c r="B226" s="325"/>
+      <c r="C226" s="303"/>
+      <c r="D226" s="301"/>
+      <c r="E226" s="302"/>
+      <c r="F226" s="302"/>
+      <c r="G226" s="302"/>
+      <c r="H226" s="302"/>
+      <c r="I226" s="302"/>
+      <c r="J226" s="302"/>
+      <c r="K226" s="303"/>
       <c r="L226" s="120"/>
     </row>
     <row r="227" spans="1:13" s="20" customFormat="1" ht="18" customHeight="1">
       <c r="A227" s="227">
         <v>10</v>
       </c>
-      <c r="B227" s="289"/>
-      <c r="C227" s="290"/>
-      <c r="D227" s="294"/>
-      <c r="E227" s="295"/>
-      <c r="F227" s="295"/>
-      <c r="G227" s="295"/>
-      <c r="H227" s="295"/>
-      <c r="I227" s="295"/>
-      <c r="J227" s="295"/>
-      <c r="K227" s="296"/>
+      <c r="B227" s="326"/>
+      <c r="C227" s="308"/>
+      <c r="D227" s="306"/>
+      <c r="E227" s="307"/>
+      <c r="F227" s="307"/>
+      <c r="G227" s="307"/>
+      <c r="H227" s="307"/>
+      <c r="I227" s="307"/>
+      <c r="J227" s="307"/>
+      <c r="K227" s="308"/>
       <c r="L227" s="122"/>
     </row>
     <row r="228" spans="1:13" ht="15" customHeight="1">
-      <c r="A228" s="272" t="s">
+      <c r="A228" s="291" t="s">
         <v>386</v>
       </c>
-      <c r="B228" s="273"/>
-      <c r="C228" s="273"/>
-      <c r="D228" s="273"/>
-      <c r="E228" s="273"/>
-      <c r="F228" s="273"/>
-      <c r="G228" s="273"/>
-      <c r="H228" s="273"/>
-      <c r="I228" s="273"/>
-      <c r="J228" s="273"/>
-      <c r="K228" s="274"/>
+      <c r="B228" s="288"/>
+      <c r="C228" s="288"/>
+      <c r="D228" s="288"/>
+      <c r="E228" s="288"/>
+      <c r="F228" s="288"/>
+      <c r="G228" s="288"/>
+      <c r="H228" s="288"/>
+      <c r="I228" s="288"/>
+      <c r="J228" s="288"/>
+      <c r="K228" s="289"/>
       <c r="L228" s="163">
         <f>SUM(L218:L227)</f>
         <v>0</v>
@@ -23216,12 +23272,67 @@
     <row r="244" spans="4:12" ht="15" customHeight="1">
       <c r="D244" s="27"/>
       <c r="E244" s="81"/>
-      <c r="J244" s="277"/>
-      <c r="K244" s="276"/>
-      <c r="L244" s="276"/>
+      <c r="J244" s="274"/>
+      <c r="K244" s="275"/>
+      <c r="L244" s="275"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="B227:C227"/>
+    <mergeCell ref="D218:K218"/>
+    <mergeCell ref="D217:K217"/>
+    <mergeCell ref="B223:C223"/>
+    <mergeCell ref="B220:C220"/>
+    <mergeCell ref="D227:K227"/>
+    <mergeCell ref="D225:K225"/>
+    <mergeCell ref="B226:C226"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="D203:K203"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="J191:L191"/>
+    <mergeCell ref="J187:L187"/>
+    <mergeCell ref="J196:L196"/>
+    <mergeCell ref="J193:L193"/>
+    <mergeCell ref="D204:K204"/>
+    <mergeCell ref="J192:L192"/>
+    <mergeCell ref="D206:K206"/>
+    <mergeCell ref="J198:L198"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="J189:L189"/>
+    <mergeCell ref="J185:L185"/>
+    <mergeCell ref="J188:L188"/>
+    <mergeCell ref="J194:L194"/>
+    <mergeCell ref="D212:K212"/>
+    <mergeCell ref="D205:K205"/>
+    <mergeCell ref="D224:K224"/>
+    <mergeCell ref="D221:K221"/>
+    <mergeCell ref="D219:K219"/>
+    <mergeCell ref="D213:K213"/>
+    <mergeCell ref="A215:L215"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="A214:K214"/>
+    <mergeCell ref="J197:L197"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="D209:K209"/>
+    <mergeCell ref="J244:L244"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="D211:K211"/>
+    <mergeCell ref="D220:K220"/>
+    <mergeCell ref="A201:L201"/>
+    <mergeCell ref="D223:K223"/>
+    <mergeCell ref="D226:K226"/>
+    <mergeCell ref="B238:L238"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="A228:K228"/>
+    <mergeCell ref="B225:C225"/>
+    <mergeCell ref="B211:C211"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="D222:K222"/>
+    <mergeCell ref="B224:C224"/>
     <mergeCell ref="D1:L1"/>
     <mergeCell ref="J190:L190"/>
     <mergeCell ref="J199:L199"/>
@@ -23238,61 +23349,6 @@
     <mergeCell ref="B206:C206"/>
     <mergeCell ref="J195:L195"/>
     <mergeCell ref="J186:L186"/>
-    <mergeCell ref="J244:L244"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="D211:K211"/>
-    <mergeCell ref="D220:K220"/>
-    <mergeCell ref="A201:L201"/>
-    <mergeCell ref="D223:K223"/>
-    <mergeCell ref="D226:K226"/>
-    <mergeCell ref="B238:L238"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="A228:K228"/>
-    <mergeCell ref="B225:C225"/>
-    <mergeCell ref="B211:C211"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="D222:K222"/>
-    <mergeCell ref="B224:C224"/>
-    <mergeCell ref="J188:L188"/>
-    <mergeCell ref="J194:L194"/>
-    <mergeCell ref="D212:K212"/>
-    <mergeCell ref="D205:K205"/>
-    <mergeCell ref="D224:K224"/>
-    <mergeCell ref="D221:K221"/>
-    <mergeCell ref="D219:K219"/>
-    <mergeCell ref="D213:K213"/>
-    <mergeCell ref="A215:L215"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="A214:K214"/>
-    <mergeCell ref="J197:L197"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="D209:K209"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="D203:K203"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="J191:L191"/>
-    <mergeCell ref="J187:L187"/>
-    <mergeCell ref="J196:L196"/>
-    <mergeCell ref="J193:L193"/>
-    <mergeCell ref="D204:K204"/>
-    <mergeCell ref="J192:L192"/>
-    <mergeCell ref="D206:K206"/>
-    <mergeCell ref="J198:L198"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="J189:L189"/>
-    <mergeCell ref="J185:L185"/>
-    <mergeCell ref="B227:C227"/>
-    <mergeCell ref="D218:K218"/>
-    <mergeCell ref="D217:K217"/>
-    <mergeCell ref="B223:C223"/>
-    <mergeCell ref="B220:C220"/>
-    <mergeCell ref="D227:K227"/>
-    <mergeCell ref="D225:K225"/>
-    <mergeCell ref="B226:C226"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0300-000000000000}">
@@ -23334,7 +23390,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -23899,42 +23955,42 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="F25" s="315" t="s">
+      <c r="F25" s="319" t="s">
         <v>499</v>
       </c>
-      <c r="G25" s="264"/>
-      <c r="H25" s="316"/>
-      <c r="I25" s="264"/>
+      <c r="G25" s="268"/>
+      <c r="H25" s="320"/>
+      <c r="I25" s="268"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="F26" s="264"/>
-      <c r="G26" s="264"/>
-      <c r="H26" s="316"/>
-      <c r="I26" s="264"/>
+      <c r="F26" s="268"/>
+      <c r="G26" s="268"/>
+      <c r="H26" s="320"/>
+      <c r="I26" s="268"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="F27" s="264"/>
-      <c r="G27" s="264"/>
-      <c r="H27" s="316"/>
-      <c r="I27" s="264"/>
+      <c r="F27" s="268"/>
+      <c r="G27" s="268"/>
+      <c r="H27" s="320"/>
+      <c r="I27" s="268"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="F28" s="264"/>
-      <c r="G28" s="264"/>
-      <c r="H28" s="316"/>
-      <c r="I28" s="264"/>
+      <c r="F28" s="268"/>
+      <c r="G28" s="268"/>
+      <c r="H28" s="320"/>
+      <c r="I28" s="268"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="F29" s="264"/>
-      <c r="G29" s="264"/>
-      <c r="H29" s="316"/>
-      <c r="I29" s="264"/>
+      <c r="F29" s="268"/>
+      <c r="G29" s="268"/>
+      <c r="H29" s="320"/>
+      <c r="I29" s="268"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="F30" s="264"/>
-      <c r="G30" s="264"/>
-      <c r="H30" s="316"/>
-      <c r="I30" s="264"/>
+      <c r="F30" s="268"/>
+      <c r="G30" s="268"/>
+      <c r="H30" s="320"/>
+      <c r="I30" s="268"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>